<commit_message>
Changed unknown names to match all case types
</commit_message>
<xml_diff>
--- a/reference/reference.xlsx
+++ b/reference/reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Programming/Python/Degenreur/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB6F88B-5B18-EF45-9EBC-9EEC2F496412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2288CCDE-FA82-2245-AE02-48BE99000AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="27300" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="740" windowWidth="27300" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Female pronouns" sheetId="1" r:id="rId1"/>
@@ -6959,8 +6959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8208,7 +8208,7 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>162</v>
+        <v>2186</v>
       </c>
       <c r="C89" t="s">
         <v>241</v>
@@ -8254,7 +8254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Search page logic now in JavaScript
</commit_message>
<xml_diff>
--- a/reference/reference.xlsx
+++ b/reference/reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Programming/Python/Degenreur/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229AA662-4363-5743-819C-382908FB7A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0551E27A-CC73-654D-B14F-84AA9167BD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="740" windowWidth="27300" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Female pronouns" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2792" uniqueCount="2299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="2305">
   <si>
     <t>Original</t>
   </si>
@@ -6920,6 +6920,24 @@
   </si>
   <si>
     <t>landlord</t>
+  </si>
+  <si>
+    <t>god</t>
+  </si>
+  <si>
+    <t>goddess</t>
+  </si>
+  <si>
+    <t>gxd</t>
+  </si>
+  <si>
+    <t>goddesses</t>
+  </si>
+  <si>
+    <t>gxds</t>
+  </si>
+  <si>
+    <t>gods</t>
   </si>
 </sst>
 </file>
@@ -7287,10 +7305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8855,6 +8873,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2303</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D113" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8862,10 +8908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10427,6 +10473,34 @@
         <v>2296</v>
       </c>
       <c r="D111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2299</v>
+      </c>
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2303</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D113" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New samples and bug fixes
</commit_message>
<xml_diff>
--- a/reference/reference.xlsx
+++ b/reference/reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Programming/Python/Degenreur/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0551E27A-CC73-654D-B14F-84AA9167BD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EC8809-5F86-8647-AC88-BA2B056586F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="18380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Female pronouns" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="2305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2863" uniqueCount="2329">
   <si>
     <t>Original</t>
   </si>
@@ -6938,6 +6938,78 @@
   </si>
   <si>
     <t>gods</t>
+  </si>
+  <si>
+    <t>maid</t>
+  </si>
+  <si>
+    <t>servant</t>
+  </si>
+  <si>
+    <t>manservant</t>
+  </si>
+  <si>
+    <t>maids</t>
+  </si>
+  <si>
+    <t>servants</t>
+  </si>
+  <si>
+    <t>manservants</t>
+  </si>
+  <si>
+    <t>brotherly</t>
+  </si>
+  <si>
+    <t>siblinglike</t>
+  </si>
+  <si>
+    <t>sisterly</t>
+  </si>
+  <si>
+    <t>girlishly</t>
+  </si>
+  <si>
+    <t>boyishly</t>
+  </si>
+  <si>
+    <t>childlikely</t>
+  </si>
+  <si>
+    <t>lady-like</t>
+  </si>
+  <si>
+    <t>ladylike</t>
+  </si>
+  <si>
+    <t>siblingly</t>
+  </si>
+  <si>
+    <t>boyish</t>
+  </si>
+  <si>
+    <t>childlike</t>
+  </si>
+  <si>
+    <t>girlish</t>
+  </si>
+  <si>
+    <t>proper</t>
+  </si>
+  <si>
+    <t>gentlemanly</t>
+  </si>
+  <si>
+    <t>unladylike</t>
+  </si>
+  <si>
+    <t>ungentlemanly</t>
+  </si>
+  <si>
+    <t>unlady-like</t>
+  </si>
+  <si>
+    <t>improper</t>
   </si>
 </sst>
 </file>
@@ -7305,10 +7377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8875,13 +8947,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>2299</v>
+        <v>2300</v>
       </c>
       <c r="B112" t="s">
         <v>2301</v>
       </c>
       <c r="C112" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -8889,15 +8961,141 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
       <c r="B113" t="s">
         <v>2303</v>
       </c>
       <c r="C113" t="s">
-        <v>2302</v>
+        <v>2304</v>
       </c>
       <c r="D113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>2305</v>
+      </c>
+      <c r="B114" t="s">
+        <v>2306</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2307</v>
+      </c>
+      <c r="D114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2309</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2310</v>
+      </c>
+      <c r="D115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>2313</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2311</v>
+      </c>
+      <c r="D116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2315</v>
+      </c>
+      <c r="D117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>2317</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2324</v>
+      </c>
+      <c r="D118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>2318</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2324</v>
+      </c>
+      <c r="D119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B121" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B122" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D122" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8908,10 +9106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G114" sqref="G114"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10478,13 +10676,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="B112" t="s">
         <v>2301</v>
       </c>
       <c r="C112" t="s">
-        <v>2299</v>
+        <v>2300</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -10492,15 +10690,85 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>2302</v>
+        <v>2304</v>
       </c>
       <c r="B113" t="s">
         <v>2303</v>
       </c>
       <c r="C113" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
       <c r="D113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B114" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2313</v>
+      </c>
+      <c r="D114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>2315</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2314</v>
+      </c>
+      <c r="D115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>2320</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>2326</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2325</v>
+      </c>
+      <c r="D118" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10513,7 +10781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C806"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
+    <sheetView topLeftCell="A90" workbookViewId="0">
       <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
@@ -16819,8 +17087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B383"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18297,123 +18565,174 @@
       <c r="A184" t="s">
         <v>1900</v>
       </c>
+      <c r="B184" t="s">
+        <v>1182</v>
+      </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>1901</v>
       </c>
+      <c r="B185" t="s">
+        <v>2238</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>1902</v>
       </c>
+      <c r="B186" t="s">
+        <v>2223</v>
+      </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>1903</v>
       </c>
+      <c r="B187" t="s">
+        <v>1394</v>
+      </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>1904</v>
       </c>
+      <c r="B188" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>1905</v>
       </c>
+      <c r="B189" t="s">
+        <v>1214</v>
+      </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>1906</v>
       </c>
+      <c r="B190" t="s">
+        <v>2238</v>
+      </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>1907</v>
       </c>
+      <c r="B191" t="s">
+        <v>2106</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>1908</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B192" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>1909</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B193" t="s">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>1910</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B194" t="s">
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>1911</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B195" t="s">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>1912</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B196" t="s">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B197" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>1857</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B198" t="s">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B199" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>1915</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B200" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>1916</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>1917</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>1918</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>1919</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>1920</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>1921</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>1922</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>1923</v>
       </c>

</xml_diff>

<commit_message>
Fixed bugs - sample downloading message
</commit_message>
<xml_diff>
--- a/reference/reference.xlsx
+++ b/reference/reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Programming/Python/Degenreur/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D45991-31A0-AE41-94E2-439B09C8549E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39FBC20-68EE-F240-B31B-FEA0E54B4C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Female pronouns" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="2334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="2392">
   <si>
     <t>Original</t>
   </si>
@@ -7025,6 +7025,180 @@
   </si>
   <si>
     <t>herr-fraulein</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>non-binary</t>
+  </si>
+  <si>
+    <t>feminine</t>
+  </si>
+  <si>
+    <t>masculine</t>
+  </si>
+  <si>
+    <t>hombre</t>
+  </si>
+  <si>
+    <t>chica</t>
+  </si>
+  <si>
+    <t>ragazzo</t>
+  </si>
+  <si>
+    <t>ragazza</t>
+  </si>
+  <si>
+    <t>tía</t>
+  </si>
+  <si>
+    <t>tío</t>
+  </si>
+  <si>
+    <t>doña</t>
+  </si>
+  <si>
+    <t>señor</t>
+  </si>
+  <si>
+    <t>señora</t>
+  </si>
+  <si>
+    <t>tíx</t>
+  </si>
+  <si>
+    <t>ragazz</t>
+  </si>
+  <si>
+    <t>señorx</t>
+  </si>
+  <si>
+    <t>chicx</t>
+  </si>
+  <si>
+    <t>dude</t>
+  </si>
+  <si>
+    <t>maternal</t>
+  </si>
+  <si>
+    <t>parental</t>
+  </si>
+  <si>
+    <t>paternal</t>
+  </si>
+  <si>
+    <t>gent</t>
+  </si>
+  <si>
+    <t>manful</t>
+  </si>
+  <si>
+    <t>manlike</t>
+  </si>
+  <si>
+    <t>womanlike</t>
+  </si>
+  <si>
+    <t>damsel</t>
+  </si>
+  <si>
+    <t>demoiselle</t>
+  </si>
+  <si>
+    <t>mademoiselle</t>
+  </si>
+  <si>
+    <t>dame</t>
+  </si>
+  <si>
+    <t>bimbo</t>
+  </si>
+  <si>
+    <t>himbo</t>
+  </si>
+  <si>
+    <t>thembo</t>
+  </si>
+  <si>
+    <t>chick</t>
+  </si>
+  <si>
+    <t>virile</t>
+  </si>
+  <si>
+    <t>virility</t>
+  </si>
+  <si>
+    <t>non-binarity</t>
+  </si>
+  <si>
+    <t>femininity</t>
+  </si>
+  <si>
+    <t>maleness</t>
+  </si>
+  <si>
+    <t>femaleness</t>
+  </si>
+  <si>
+    <t>manhood</t>
+  </si>
+  <si>
+    <t>womanhood</t>
+  </si>
+  <si>
+    <t>personhood</t>
+  </si>
+  <si>
+    <t>girlishness</t>
+  </si>
+  <si>
+    <t>boyishness</t>
+  </si>
+  <si>
+    <t>youth</t>
+  </si>
+  <si>
+    <t>mannish</t>
+  </si>
+  <si>
+    <t>macho</t>
+  </si>
+  <si>
+    <t>butch</t>
+  </si>
+  <si>
+    <t>androgynous</t>
+  </si>
+  <si>
+    <t>tomboy</t>
+  </si>
+  <si>
+    <t>femboy</t>
+  </si>
+  <si>
+    <t>androgyne</t>
+  </si>
+  <si>
+    <t>machismo</t>
+  </si>
+  <si>
+    <t>butchness</t>
+  </si>
+  <si>
+    <t>androgynity</t>
+  </si>
+  <si>
+    <t>gents</t>
+  </si>
+  <si>
+    <t>gentlefolk</t>
   </si>
 </sst>
 </file>
@@ -7392,10 +7566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D125"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7422,13 +7596,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -7436,13 +7610,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -7450,13 +7624,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -7464,13 +7638,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -7478,13 +7652,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -7492,13 +7666,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -7506,13 +7680,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -7520,13 +7694,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>229</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -7534,13 +7708,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -7548,13 +7722,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>2364</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>2366</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>2365</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -7562,13 +7736,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>233</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -7576,13 +7750,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>234</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -7590,13 +7764,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>235</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -7604,13 +7778,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>157</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>236</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -7618,13 +7792,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
+        <v>209</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -7632,27 +7806,27 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>2175</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>2176</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>2177</v>
+        <v>210</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>2382</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>2383</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>2381</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -7660,13 +7834,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2266</v>
+        <v>2388</v>
       </c>
       <c r="B19" t="s">
-        <v>2268</v>
+        <v>2389</v>
       </c>
       <c r="C19" t="s">
-        <v>2267</v>
+        <v>2387</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -7674,13 +7848,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>2340</v>
       </c>
       <c r="B20" t="s">
-        <v>2329</v>
+        <v>2351</v>
       </c>
       <c r="C20" t="s">
-        <v>175</v>
+        <v>2339</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -7688,13 +7862,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>2271</v>
       </c>
       <c r="B21" t="s">
-        <v>2329</v>
+        <v>2270</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>2269</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -7702,13 +7876,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>2272</v>
       </c>
       <c r="B22" t="s">
-        <v>2328</v>
+        <v>2273</v>
       </c>
       <c r="C22" t="s">
-        <v>176</v>
+        <v>2274</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -7716,13 +7890,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>2328</v>
+        <v>137</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -7730,13 +7904,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>264</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>2330</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -7744,13 +7918,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2331</v>
+        <v>2264</v>
       </c>
       <c r="B25" t="s">
-        <v>2330</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
+        <v>2265</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -7758,13 +7932,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>2329</v>
+        <v>138</v>
       </c>
       <c r="C26" t="s">
-        <v>177</v>
+        <v>216</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -7772,13 +7946,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>257</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -7786,13 +7960,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>2363</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -7800,13 +7974,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>2360</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>2356</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -7814,13 +7988,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -7828,13 +8002,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -7842,13 +8016,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>2361</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -7856,13 +8030,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>2345</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>2350</v>
       </c>
       <c r="C33" t="s">
-        <v>178</v>
+        <v>2346</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -7870,13 +8044,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="C34" t="s">
-        <v>179</v>
+        <v>230</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -7884,13 +8058,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>2352</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>2352</v>
       </c>
       <c r="C35" t="s">
-        <v>184</v>
+        <v>2367</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -7898,13 +8072,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>2240</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>2239</v>
       </c>
       <c r="C36" t="s">
-        <v>185</v>
+        <v>2238</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -7912,13 +8086,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>2243</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>2242</v>
       </c>
       <c r="C37" t="s">
-        <v>186</v>
+        <v>2241</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -7926,13 +8100,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>2334</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>2336</v>
       </c>
       <c r="C38" t="s">
-        <v>187</v>
+        <v>2335</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -7940,13 +8114,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>2373</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>2370</v>
       </c>
       <c r="C39" t="s">
-        <v>188</v>
+        <v>2372</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -7954,13 +8128,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>2337</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>2336</v>
       </c>
       <c r="C40" t="s">
-        <v>189</v>
+        <v>2338</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -7968,13 +8142,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>2371</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>2370</v>
       </c>
       <c r="C41" t="s">
-        <v>190</v>
+        <v>2369</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -7982,13 +8156,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -7996,13 +8170,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>2252</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>2251</v>
       </c>
       <c r="C43" t="s">
-        <v>192</v>
+        <v>2250</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -8010,13 +8184,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>2332</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>2333</v>
       </c>
       <c r="C44" t="s">
-        <v>193</v>
+        <v>2250</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -8024,13 +8198,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>2246</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>2245</v>
       </c>
       <c r="C45" t="s">
-        <v>194</v>
+        <v>2244</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -8038,13 +8212,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>2248</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>2249</v>
       </c>
       <c r="C46" t="s">
-        <v>194</v>
+        <v>2247</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -8052,13 +8226,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -8066,13 +8240,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -8080,13 +8254,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>257</v>
       </c>
       <c r="C49" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -8094,13 +8268,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C50" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -8108,13 +8282,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>121</v>
+        <v>196</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -8122,13 +8296,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -8136,13 +8310,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -8150,13 +8324,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>2318</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>2317</v>
       </c>
       <c r="C54" t="s">
-        <v>201</v>
+        <v>2316</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -8164,13 +8338,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>2310</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>2312</v>
       </c>
       <c r="C55" t="s">
-        <v>202</v>
+        <v>2311</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -8178,13 +8352,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>2377</v>
       </c>
       <c r="B56" t="s">
-        <v>126</v>
+        <v>2379</v>
       </c>
       <c r="C56" t="s">
-        <v>203</v>
+        <v>2378</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -8192,13 +8366,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
       <c r="C57" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -8206,13 +8380,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C58" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -8220,13 +8394,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -8234,13 +8408,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>2296</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>2297</v>
       </c>
       <c r="C60" t="s">
-        <v>207</v>
+        <v>2295</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -8248,13 +8422,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>2298</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>2299</v>
       </c>
       <c r="C61" t="s">
-        <v>208</v>
+        <v>2300</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -8262,13 +8436,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C62" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
@@ -8276,13 +8450,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C63" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -8290,13 +8464,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -8304,13 +8478,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -8318,13 +8492,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -8332,13 +8506,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="C67" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -8346,13 +8520,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -8360,13 +8534,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C69" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -8374,13 +8548,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="C70" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -8388,13 +8562,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -8402,13 +8576,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="C72" t="s">
-        <v>219</v>
+        <v>162</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -8416,13 +8590,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C73" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D73" t="b">
         <v>1</v>
@@ -8430,13 +8604,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C74" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -8444,13 +8618,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
@@ -8458,13 +8632,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
@@ -8500,13 +8674,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="C79" t="s">
-        <v>226</v>
+        <v>185</v>
       </c>
       <c r="D79" t="b">
         <v>1</v>
@@ -8514,13 +8688,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B80" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -8528,13 +8702,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>2313</v>
       </c>
       <c r="B81" t="s">
-        <v>149</v>
+        <v>2319</v>
       </c>
       <c r="C81" t="s">
-        <v>228</v>
+        <v>2320</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
@@ -8542,13 +8716,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>2314</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>2319</v>
       </c>
       <c r="C82" t="s">
-        <v>229</v>
+        <v>2320</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -8556,13 +8730,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>2292</v>
       </c>
       <c r="B83" t="s">
-        <v>149</v>
+        <v>2293</v>
       </c>
       <c r="C83" t="s">
-        <v>230</v>
+        <v>2294</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -8570,13 +8744,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>2287</v>
       </c>
       <c r="B84" t="s">
-        <v>151</v>
+        <v>2289</v>
       </c>
       <c r="C84" t="s">
-        <v>231</v>
+        <v>2288</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
@@ -8584,13 +8758,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>2290</v>
       </c>
       <c r="B85" t="s">
-        <v>152</v>
+        <v>257</v>
       </c>
       <c r="C85" t="s">
-        <v>232</v>
+        <v>2291</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -8598,13 +8772,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>2261</v>
       </c>
       <c r="B86" t="s">
-        <v>153</v>
+        <v>2262</v>
       </c>
       <c r="C86" t="s">
-        <v>84</v>
+        <v>2263</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -8612,13 +8786,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="B87" t="s">
-        <v>154</v>
+        <v>2329</v>
       </c>
       <c r="C87" t="s">
-        <v>233</v>
+        <v>177</v>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -8626,13 +8800,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="B88" t="s">
-        <v>155</v>
+        <v>2328</v>
       </c>
       <c r="C88" t="s">
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="D88" t="b">
         <v>1</v>
@@ -8640,13 +8814,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B89" t="s">
-        <v>156</v>
+        <v>2328</v>
       </c>
       <c r="C89" t="s">
-        <v>235</v>
+        <v>176</v>
       </c>
       <c r="D89" t="b">
         <v>1</v>
@@ -8654,13 +8828,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="B90" t="s">
-        <v>157</v>
+        <v>2253</v>
       </c>
       <c r="C90" t="s">
-        <v>236</v>
+        <v>176</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -8668,13 +8842,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>2331</v>
       </c>
       <c r="B91" t="s">
-        <v>2178</v>
+        <v>2330</v>
       </c>
       <c r="C91" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -8682,13 +8856,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="B92" t="s">
-        <v>159</v>
+        <v>2330</v>
       </c>
       <c r="C92" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D92" t="b">
         <v>1</v>
@@ -8696,13 +8870,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>2362</v>
       </c>
       <c r="B93" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
       <c r="C93" t="s">
-        <v>239</v>
+        <v>184</v>
       </c>
       <c r="D93" t="b">
         <v>1</v>
@@ -8710,13 +8884,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>2240</v>
+        <v>2301</v>
       </c>
       <c r="B94" t="s">
-        <v>2239</v>
+        <v>2302</v>
       </c>
       <c r="C94" t="s">
-        <v>2238</v>
+        <v>2303</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -8724,13 +8898,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>2243</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s">
-        <v>2242</v>
+        <v>107</v>
       </c>
       <c r="C95" t="s">
-        <v>2241</v>
+        <v>182</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -8738,13 +8912,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>2246</v>
+        <v>30</v>
       </c>
       <c r="B96" t="s">
-        <v>2245</v>
+        <v>108</v>
       </c>
       <c r="C96" t="s">
-        <v>2244</v>
+        <v>183</v>
       </c>
       <c r="D96" t="b">
         <v>1</v>
@@ -8752,13 +8926,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>2248</v>
+        <v>2304</v>
       </c>
       <c r="B97" t="s">
-        <v>2249</v>
+        <v>2305</v>
       </c>
       <c r="C97" t="s">
-        <v>2247</v>
+        <v>2306</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -8766,13 +8940,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>2252</v>
+        <v>12</v>
       </c>
       <c r="B98" t="s">
-        <v>2251</v>
+        <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>2250</v>
+        <v>168</v>
       </c>
       <c r="D98" t="b">
         <v>1</v>
@@ -8780,13 +8954,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>2332</v>
+        <v>14</v>
       </c>
       <c r="B99" t="s">
-        <v>2333</v>
+        <v>100</v>
       </c>
       <c r="C99" t="s">
-        <v>2250</v>
+        <v>170</v>
       </c>
       <c r="D99" t="b">
         <v>1</v>
@@ -8794,13 +8968,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>22</v>
+        <v>2353</v>
       </c>
       <c r="B100" t="s">
-        <v>2253</v>
+        <v>2354</v>
       </c>
       <c r="C100" t="s">
-        <v>176</v>
+        <v>2355</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -8808,27 +8982,27 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>2256</v>
+        <v>2175</v>
       </c>
       <c r="B101" t="s">
-        <v>2255</v>
+        <v>2176</v>
       </c>
       <c r="C101" t="s">
-        <v>2254</v>
+        <v>2177</v>
       </c>
       <c r="D101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>2257</v>
+        <v>21</v>
       </c>
       <c r="B102" t="s">
-        <v>2258</v>
+        <v>2329</v>
       </c>
       <c r="C102" t="s">
-        <v>2259</v>
+        <v>175</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -8836,13 +9010,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>2260</v>
+        <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>2258</v>
+        <v>2329</v>
       </c>
       <c r="C103" t="s">
-        <v>2259</v>
+        <v>175</v>
       </c>
       <c r="D103" t="b">
         <v>1</v>
@@ -8850,13 +9024,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>2261</v>
+        <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>2262</v>
+        <v>104</v>
       </c>
       <c r="C104" t="s">
-        <v>2263</v>
+        <v>175</v>
       </c>
       <c r="D104" t="b">
         <v>1</v>
@@ -8864,13 +9038,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>2264</v>
+        <v>2266</v>
       </c>
       <c r="B105" t="s">
-        <v>151</v>
+        <v>2268</v>
       </c>
       <c r="C105" t="s">
-        <v>2265</v>
+        <v>2267</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -8878,13 +9052,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>2271</v>
+        <v>13</v>
       </c>
       <c r="B106" t="s">
-        <v>2270</v>
+        <v>100</v>
       </c>
       <c r="C106" t="s">
-        <v>2269</v>
+        <v>169</v>
       </c>
       <c r="D106" t="b">
         <v>1</v>
@@ -8892,13 +9066,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>2272</v>
+        <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>2273</v>
+        <v>98</v>
       </c>
       <c r="C107" t="s">
-        <v>2274</v>
+        <v>166</v>
       </c>
       <c r="D107" t="b">
         <v>1</v>
@@ -8906,13 +9080,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>2276</v>
+        <v>2282</v>
       </c>
       <c r="B108" t="s">
-        <v>2279</v>
+        <v>2283</v>
       </c>
       <c r="C108" t="s">
-        <v>2275</v>
+        <v>2281</v>
       </c>
       <c r="D108" t="b">
         <v>1</v>
@@ -8920,13 +9094,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>2278</v>
+        <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>2280</v>
+        <v>99</v>
       </c>
       <c r="C109" t="s">
-        <v>2277</v>
+        <v>167</v>
       </c>
       <c r="D109" t="b">
         <v>1</v>
@@ -8934,13 +9108,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>2282</v>
+        <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>2283</v>
+        <v>104</v>
       </c>
       <c r="C110" t="s">
-        <v>2281</v>
+        <v>174</v>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -8948,13 +9122,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>2287</v>
+        <v>37</v>
       </c>
       <c r="B111" t="s">
-        <v>2289</v>
+        <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>2288</v>
+        <v>188</v>
       </c>
       <c r="D111" t="b">
         <v>1</v>
@@ -8962,13 +9136,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>2290</v>
+        <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>257</v>
+        <v>114</v>
       </c>
       <c r="C112" t="s">
-        <v>2291</v>
+        <v>189</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -8976,13 +9150,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>2292</v>
+        <v>64</v>
       </c>
       <c r="B113" t="s">
-        <v>2293</v>
+        <v>136</v>
       </c>
       <c r="C113" t="s">
-        <v>2294</v>
+        <v>213</v>
       </c>
       <c r="D113" t="b">
         <v>1</v>
@@ -8990,13 +9164,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>2296</v>
+        <v>82</v>
       </c>
       <c r="B114" t="s">
-        <v>2297</v>
+        <v>151</v>
       </c>
       <c r="C114" t="s">
-        <v>2295</v>
+        <v>231</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -9004,13 +9178,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>2298</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>2299</v>
+        <v>152</v>
       </c>
       <c r="C115" t="s">
-        <v>2300</v>
+        <v>232</v>
       </c>
       <c r="D115" t="b">
         <v>1</v>
@@ -9018,13 +9192,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>2301</v>
+        <v>62</v>
       </c>
       <c r="B116" t="s">
-        <v>2302</v>
+        <v>134</v>
       </c>
       <c r="C116" t="s">
-        <v>2303</v>
+        <v>211</v>
       </c>
       <c r="D116" t="b">
         <v>1</v>
@@ -9032,13 +9206,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>2304</v>
+        <v>63</v>
       </c>
       <c r="B117" t="s">
-        <v>2305</v>
+        <v>135</v>
       </c>
       <c r="C117" t="s">
-        <v>2306</v>
+        <v>212</v>
       </c>
       <c r="D117" t="b">
         <v>1</v>
@@ -9046,13 +9220,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>2309</v>
+        <v>2342</v>
       </c>
       <c r="B118" t="s">
-        <v>2308</v>
+        <v>2349</v>
       </c>
       <c r="C118" t="s">
-        <v>2307</v>
+        <v>2341</v>
       </c>
       <c r="D118" t="b">
         <v>1</v>
@@ -9060,13 +9234,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>2310</v>
+        <v>90</v>
       </c>
       <c r="B119" t="s">
-        <v>2312</v>
+        <v>159</v>
       </c>
       <c r="C119" t="s">
-        <v>2311</v>
+        <v>238</v>
       </c>
       <c r="D119" t="b">
         <v>1</v>
@@ -9074,13 +9248,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>2313</v>
+        <v>91</v>
       </c>
       <c r="B120" t="s">
-        <v>2319</v>
+        <v>160</v>
       </c>
       <c r="C120" t="s">
-        <v>2320</v>
+        <v>239</v>
       </c>
       <c r="D120" t="b">
         <v>1</v>
@@ -9088,13 +9262,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>2314</v>
+        <v>89</v>
       </c>
       <c r="B121" t="s">
-        <v>2319</v>
+        <v>2178</v>
       </c>
       <c r="C121" t="s">
-        <v>2320</v>
+        <v>237</v>
       </c>
       <c r="D121" t="b">
         <v>1</v>
@@ -9102,13 +9276,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>2318</v>
+        <v>2256</v>
       </c>
       <c r="B122" t="s">
-        <v>2317</v>
+        <v>2255</v>
       </c>
       <c r="C122" t="s">
-        <v>2316</v>
+        <v>2254</v>
       </c>
       <c r="D122" t="b">
         <v>1</v>
@@ -9116,13 +9290,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>2321</v>
+        <v>4</v>
       </c>
       <c r="B123" t="s">
-        <v>2324</v>
+        <v>92</v>
       </c>
       <c r="C123" t="s">
-        <v>2322</v>
+        <v>161</v>
       </c>
       <c r="D123" t="b">
         <v>1</v>
@@ -9130,13 +9304,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>2323</v>
+        <v>2257</v>
       </c>
       <c r="B124" t="s">
-        <v>2324</v>
+        <v>2258</v>
       </c>
       <c r="C124" t="s">
-        <v>2322</v>
+        <v>2259</v>
       </c>
       <c r="D124" t="b">
         <v>1</v>
@@ -9144,29 +9318,340 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B125" t="s">
+        <v>2258</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" t="s">
+        <v>103</v>
+      </c>
+      <c r="C126" t="s">
+        <v>173</v>
+      </c>
+      <c r="D126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>15</v>
+      </c>
+      <c r="B127" t="s">
+        <v>101</v>
+      </c>
+      <c r="C127" t="s">
+        <v>171</v>
+      </c>
+      <c r="D127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2307</v>
+      </c>
+      <c r="D128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>16</v>
+      </c>
+      <c r="B129" t="s">
+        <v>102</v>
+      </c>
+      <c r="C129" t="s">
+        <v>172</v>
+      </c>
+      <c r="D129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>71</v>
+      </c>
+      <c r="B130" t="s">
+        <v>142</v>
+      </c>
+      <c r="C130" t="s">
+        <v>220</v>
+      </c>
+      <c r="D130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" t="s">
+        <v>143</v>
+      </c>
+      <c r="C131" t="s">
+        <v>221</v>
+      </c>
+      <c r="D131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>2343</v>
+      </c>
+      <c r="B132" t="s">
+        <v>2348</v>
+      </c>
+      <c r="C132" t="s">
+        <v>2344</v>
+      </c>
+      <c r="D132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>2384</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2385</v>
+      </c>
+      <c r="D133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>2323</v>
+      </c>
+      <c r="B134" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C134" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>2321</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C135" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>77</v>
+      </c>
+      <c r="B136" t="s">
+        <v>148</v>
+      </c>
+      <c r="C136" t="s">
+        <v>226</v>
+      </c>
+      <c r="D136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>78</v>
+      </c>
+      <c r="B137" t="s">
+        <v>148</v>
+      </c>
+      <c r="C137" t="s">
+        <v>227</v>
+      </c>
+      <c r="D137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>47</v>
+      </c>
+      <c r="B138" t="s">
+        <v>119</v>
+      </c>
+      <c r="C138" t="s">
+        <v>197</v>
+      </c>
+      <c r="D138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2279</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2275</v>
+      </c>
+      <c r="D139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B140" t="s">
+        <v>2280</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2277</v>
+      </c>
+      <c r="D140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>48</v>
+      </c>
+      <c r="B141" t="s">
+        <v>120</v>
+      </c>
+      <c r="C141" t="s">
+        <v>198</v>
+      </c>
+      <c r="D141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" t="s">
+        <v>96</v>
+      </c>
+      <c r="C142" t="s">
+        <v>164</v>
+      </c>
+      <c r="D142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>2375</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2376</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2374</v>
+      </c>
+      <c r="D143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>2359</v>
+      </c>
+      <c r="B144" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C144" t="s">
+        <v>2358</v>
+      </c>
+      <c r="D144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>2325</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B145" t="s">
         <v>2327</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C145" t="s">
         <v>2326</v>
       </c>
-      <c r="D125" t="b">
+      <c r="D145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B146" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>9</v>
+      </c>
+      <c r="B147" t="s">
+        <v>97</v>
+      </c>
+      <c r="C147" t="s">
+        <v>165</v>
+      </c>
+      <c r="D147" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D147">
+    <sortCondition ref="A2:A147"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9193,13 +9678,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -9207,13 +9692,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -9221,13 +9706,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -9235,13 +9720,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -9249,13 +9734,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -9263,13 +9748,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -9277,13 +9762,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>2286</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>2289</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>2287</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -9291,13 +9776,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>257</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -9305,27 +9790,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -9333,13 +9818,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -9347,13 +9832,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -9361,13 +9846,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>2316</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>2317</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>2318</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -9375,13 +9860,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>2311</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>2312</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>2310</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -9389,13 +9874,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>2378</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>2379</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>2377</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -9403,13 +9888,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -9417,13 +9902,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
-        <v>2328</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -9431,13 +9916,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B19" t="s">
-        <v>2330</v>
+        <v>256</v>
       </c>
       <c r="C19" t="s">
-        <v>264</v>
+        <v>16</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -9445,13 +9930,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
-        <v>2328</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -9459,13 +9944,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>2267</v>
+        <v>2307</v>
       </c>
       <c r="B21" t="s">
-        <v>2330</v>
+        <v>2315</v>
       </c>
       <c r="C21" t="s">
-        <v>264</v>
+        <v>2309</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -9473,13 +9958,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
-        <v>257</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -9487,13 +9972,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="B23" t="s">
-        <v>258</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -9501,13 +9986,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -9515,13 +10000,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>2288</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>2289</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>2287</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -9529,13 +10014,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>2291</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>257</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>2290</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -9543,13 +10028,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>2269</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>2270</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>2271</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -9557,13 +10042,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>244</v>
+        <v>2274</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>2273</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>2272</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -9571,13 +10056,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -9585,13 +10070,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -9599,13 +10084,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -9613,13 +10098,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -9627,13 +10112,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -9641,13 +10126,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
       <c r="B34" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>266</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -9655,13 +10140,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>189</v>
+        <v>2238</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>2239</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>2240</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -9669,13 +10154,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>190</v>
+        <v>2241</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>2242</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>2243</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -9683,13 +10168,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -9697,13 +10182,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>192</v>
+        <v>2281</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>2283</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>2282</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -9711,13 +10196,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -9725,13 +10210,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>2385</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>2386</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>2384</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -9739,13 +10224,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>2244</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>2245</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>2246</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -9753,13 +10238,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>2247</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>2249</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>2248</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -9767,13 +10252,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>2356</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -9781,13 +10266,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>2391</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -9795,13 +10280,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>2320</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>2319</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>2314</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -9809,13 +10294,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>2391</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -9823,13 +10308,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>2390</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>2391</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -9837,13 +10322,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>203</v>
+        <v>2295</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>2297</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>2296</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -9851,13 +10336,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -9865,13 +10350,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -9879,13 +10364,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>2300</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>2299</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>2298</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -9893,13 +10378,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -9907,13 +10392,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -9921,13 +10406,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -9935,13 +10420,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -9949,13 +10434,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -9963,13 +10448,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -9977,13 +10462,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>246</v>
+        <v>205</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C58" t="s">
-        <v>265</v>
+        <v>56</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -9991,13 +10476,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -10005,13 +10490,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -10019,13 +10504,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -10033,13 +10518,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="B62" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
@@ -10047,13 +10532,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>217</v>
+        <v>161</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -10061,13 +10546,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -10075,13 +10560,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -10089,13 +10574,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>220</v>
+        <v>2250</v>
       </c>
       <c r="B66" t="s">
-        <v>142</v>
+        <v>2251</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>2252</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -10103,13 +10588,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>255</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -10117,13 +10602,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>2365</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>2366</v>
       </c>
       <c r="C68" t="s">
-        <v>73</v>
+        <v>2364</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -10131,13 +10616,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="C69" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -10145,13 +10630,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="C70" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -10159,13 +10644,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>225</v>
+        <v>2339</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>2351</v>
       </c>
       <c r="C71" t="s">
-        <v>76</v>
+        <v>2340</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -10173,13 +10658,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C72" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -10187,13 +10672,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C73" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D73" t="b">
         <v>1</v>
@@ -10201,13 +10686,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>230</v>
+        <v>197</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="C74" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -10215,13 +10700,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
-        <v>266</v>
+        <v>48</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
@@ -10229,13 +10714,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C76" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
@@ -10243,13 +10728,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C77" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
@@ -10257,13 +10742,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>248</v>
+        <v>182</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
@@ -10271,13 +10756,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>2236</v>
+        <v>244</v>
       </c>
       <c r="B79" t="s">
-        <v>2237</v>
+        <v>107</v>
       </c>
       <c r="C79" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D79" t="b">
         <v>1</v>
@@ -10285,13 +10770,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="C80" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -10299,13 +10784,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="C81" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
@@ -10313,13 +10798,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>238</v>
+        <v>2294</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>2293</v>
       </c>
       <c r="C82" t="s">
-        <v>90</v>
+        <v>2292</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -10327,13 +10812,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>239</v>
+        <v>2263</v>
       </c>
       <c r="B83" t="s">
-        <v>160</v>
+        <v>2262</v>
       </c>
       <c r="C83" t="s">
-        <v>91</v>
+        <v>2261</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -10341,13 +10826,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>237</v>
+        <v>2236</v>
       </c>
       <c r="B84" t="s">
-        <v>2178</v>
+        <v>2237</v>
       </c>
       <c r="C84" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
@@ -10355,13 +10840,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>2179</v>
+        <v>2387</v>
       </c>
       <c r="B85" t="s">
-        <v>158</v>
+        <v>2389</v>
       </c>
       <c r="C85" t="s">
-        <v>2180</v>
+        <v>2388</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -10369,13 +10854,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>249</v>
+        <v>2381</v>
       </c>
       <c r="B86" t="s">
-        <v>259</v>
+        <v>2383</v>
       </c>
       <c r="C86" t="s">
-        <v>267</v>
+        <v>2382</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -10383,13 +10868,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B87" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C87" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -10397,13 +10882,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B88" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C88" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D88" t="b">
         <v>1</v>
@@ -10411,13 +10896,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>252</v>
+        <v>2335</v>
       </c>
       <c r="B89" t="s">
-        <v>261</v>
+        <v>2336</v>
       </c>
       <c r="C89" t="s">
-        <v>270</v>
+        <v>2334</v>
       </c>
       <c r="D89" t="b">
         <v>1</v>
@@ -10425,13 +10910,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>253</v>
+        <v>2372</v>
       </c>
       <c r="B90" t="s">
-        <v>262</v>
+        <v>2370</v>
       </c>
       <c r="C90" t="s">
-        <v>271</v>
+        <v>2373</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -10439,13 +10924,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>254</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>263</v>
+        <v>96</v>
       </c>
       <c r="C91" t="s">
-        <v>272</v>
+        <v>8</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -10453,13 +10938,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>2238</v>
+        <v>2357</v>
       </c>
       <c r="B92" t="s">
-        <v>2239</v>
+        <v>2336</v>
       </c>
       <c r="C92" t="s">
-        <v>2240</v>
+        <v>2325</v>
       </c>
       <c r="D92" t="b">
         <v>1</v>
@@ -10467,13 +10952,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>2241</v>
+        <v>2374</v>
       </c>
       <c r="B93" t="s">
-        <v>2242</v>
+        <v>2376</v>
       </c>
       <c r="C93" t="s">
-        <v>2243</v>
+        <v>2375</v>
       </c>
       <c r="D93" t="b">
         <v>1</v>
@@ -10481,13 +10966,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>2244</v>
+        <v>2358</v>
       </c>
       <c r="B94" t="s">
-        <v>2245</v>
+        <v>2336</v>
       </c>
       <c r="C94" t="s">
-        <v>2246</v>
+        <v>2359</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -10495,13 +10980,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>2247</v>
+        <v>2326</v>
       </c>
       <c r="B95" t="s">
-        <v>2249</v>
+        <v>2336</v>
       </c>
       <c r="C95" t="s">
-        <v>2248</v>
+        <v>2325</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -10509,13 +10994,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>2250</v>
+        <v>2380</v>
       </c>
       <c r="B96" t="s">
-        <v>2251</v>
+        <v>2336</v>
       </c>
       <c r="C96" t="s">
-        <v>2252</v>
+        <v>2325</v>
       </c>
       <c r="D96" t="b">
         <v>1</v>
@@ -10523,13 +11008,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>176</v>
+        <v>2338</v>
       </c>
       <c r="B97" t="s">
-        <v>2253</v>
+        <v>2336</v>
       </c>
       <c r="C97" t="s">
-        <v>22</v>
+        <v>2337</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -10537,13 +11022,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>2254</v>
+        <v>2284</v>
       </c>
       <c r="B98" t="s">
-        <v>2255</v>
+        <v>2285</v>
       </c>
       <c r="C98" t="s">
-        <v>2256</v>
+        <v>19</v>
       </c>
       <c r="D98" t="b">
         <v>1</v>
@@ -10551,13 +11036,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>2257</v>
+        <v>165</v>
       </c>
       <c r="B99" t="s">
-        <v>2258</v>
+        <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>2259</v>
+        <v>9</v>
       </c>
       <c r="D99" t="b">
         <v>1</v>
@@ -10565,13 +11050,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>2260</v>
+        <v>251</v>
       </c>
       <c r="B100" t="s">
-        <v>2258</v>
+        <v>261</v>
       </c>
       <c r="C100" t="s">
-        <v>2259</v>
+        <v>269</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -10579,13 +11064,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>2263</v>
+        <v>252</v>
       </c>
       <c r="B101" t="s">
-        <v>2262</v>
+        <v>261</v>
       </c>
       <c r="C101" t="s">
-        <v>2261</v>
+        <v>270</v>
       </c>
       <c r="D101" t="b">
         <v>1</v>
@@ -10593,13 +11078,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>2269</v>
+        <v>175</v>
       </c>
       <c r="B102" t="s">
-        <v>2270</v>
+        <v>2328</v>
       </c>
       <c r="C102" t="s">
-        <v>2271</v>
+        <v>23</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -10607,13 +11092,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>2274</v>
+        <v>2267</v>
       </c>
       <c r="B103" t="s">
-        <v>2273</v>
+        <v>2330</v>
       </c>
       <c r="C103" t="s">
-        <v>2272</v>
+        <v>264</v>
       </c>
       <c r="D103" t="b">
         <v>1</v>
@@ -10621,13 +11106,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>2275</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>2279</v>
+        <v>2253</v>
       </c>
       <c r="C104" t="s">
-        <v>2276</v>
+        <v>22</v>
       </c>
       <c r="D104" t="b">
         <v>1</v>
@@ -10635,13 +11120,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>2277</v>
+        <v>174</v>
       </c>
       <c r="B105" t="s">
-        <v>2280</v>
+        <v>104</v>
       </c>
       <c r="C105" t="s">
-        <v>2278</v>
+        <v>18</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -10649,13 +11134,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>2281</v>
+        <v>188</v>
       </c>
       <c r="B106" t="s">
-        <v>2283</v>
+        <v>113</v>
       </c>
       <c r="C106" t="s">
-        <v>2282</v>
+        <v>37</v>
       </c>
       <c r="D106" t="b">
         <v>1</v>
@@ -10663,13 +11148,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>2284</v>
+        <v>189</v>
       </c>
       <c r="B107" t="s">
-        <v>2285</v>
+        <v>114</v>
       </c>
       <c r="C107" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D107" t="b">
         <v>1</v>
@@ -10677,13 +11162,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>2286</v>
+        <v>168</v>
       </c>
       <c r="B108" t="s">
-        <v>2289</v>
+        <v>100</v>
       </c>
       <c r="C108" t="s">
-        <v>2287</v>
+        <v>12</v>
       </c>
       <c r="D108" t="b">
         <v>1</v>
@@ -10691,13 +11176,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>2288</v>
+        <v>2355</v>
       </c>
       <c r="B109" t="s">
-        <v>2289</v>
+        <v>2354</v>
       </c>
       <c r="C109" t="s">
-        <v>2287</v>
+        <v>2353</v>
       </c>
       <c r="D109" t="b">
         <v>1</v>
@@ -10705,13 +11190,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>2291</v>
+        <v>170</v>
       </c>
       <c r="B110" t="s">
-        <v>257</v>
+        <v>100</v>
       </c>
       <c r="C110" t="s">
-        <v>2290</v>
+        <v>14</v>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -10719,27 +11204,27 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>2294</v>
+        <v>241</v>
       </c>
       <c r="B111" t="s">
-        <v>2293</v>
+        <v>100</v>
       </c>
       <c r="C111" t="s">
-        <v>2292</v>
+        <v>13</v>
       </c>
       <c r="D111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>2295</v>
+        <v>246</v>
       </c>
       <c r="B112" t="s">
-        <v>2297</v>
+        <v>137</v>
       </c>
       <c r="C112" t="s">
-        <v>2296</v>
+        <v>265</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -10747,13 +11232,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>2300</v>
+        <v>213</v>
       </c>
       <c r="B113" t="s">
-        <v>2299</v>
+        <v>137</v>
       </c>
       <c r="C113" t="s">
-        <v>2298</v>
+        <v>64</v>
       </c>
       <c r="D113" t="b">
         <v>1</v>
@@ -10761,13 +11246,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>2307</v>
+        <v>231</v>
       </c>
       <c r="B114" t="s">
-        <v>2315</v>
+        <v>151</v>
       </c>
       <c r="C114" t="s">
-        <v>2309</v>
+        <v>82</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -10775,13 +11260,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>2311</v>
+        <v>232</v>
       </c>
       <c r="B115" t="s">
-        <v>2312</v>
+        <v>152</v>
       </c>
       <c r="C115" t="s">
-        <v>2310</v>
+        <v>83</v>
       </c>
       <c r="D115" t="b">
         <v>1</v>
@@ -10789,13 +11274,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>2316</v>
+        <v>2341</v>
       </c>
       <c r="B116" t="s">
-        <v>2317</v>
+        <v>2349</v>
       </c>
       <c r="C116" t="s">
-        <v>2318</v>
+        <v>2342</v>
       </c>
       <c r="D116" t="b">
         <v>1</v>
@@ -10803,13 +11288,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>2320</v>
+        <v>253</v>
       </c>
       <c r="B117" t="s">
-        <v>2319</v>
+        <v>262</v>
       </c>
       <c r="C117" t="s">
-        <v>2314</v>
+        <v>271</v>
       </c>
       <c r="D117" t="b">
         <v>1</v>
@@ -10817,13 +11302,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>2322</v>
+        <v>254</v>
       </c>
       <c r="B118" t="s">
-        <v>2324</v>
+        <v>263</v>
       </c>
       <c r="C118" t="s">
-        <v>2321</v>
+        <v>272</v>
       </c>
       <c r="D118" t="b">
         <v>1</v>
@@ -10831,19 +11316,316 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>2326</v>
+        <v>238</v>
       </c>
       <c r="B119" t="s">
-        <v>2327</v>
+        <v>159</v>
       </c>
       <c r="C119" t="s">
-        <v>2325</v>
+        <v>90</v>
       </c>
       <c r="D119" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>239</v>
+      </c>
+      <c r="B120" t="s">
+        <v>160</v>
+      </c>
+      <c r="C120" t="s">
+        <v>91</v>
+      </c>
+      <c r="D120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>237</v>
+      </c>
+      <c r="B121" t="s">
+        <v>2178</v>
+      </c>
+      <c r="C121" t="s">
+        <v>89</v>
+      </c>
+      <c r="D121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>2179</v>
+      </c>
+      <c r="B122" t="s">
+        <v>158</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B123" t="s">
+        <v>2255</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2256</v>
+      </c>
+      <c r="D123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2350</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2347</v>
+      </c>
+      <c r="D124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>2257</v>
+      </c>
+      <c r="B125" t="s">
+        <v>2258</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B126" t="s">
+        <v>2258</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>177</v>
+      </c>
+      <c r="B127" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C127" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>243</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2330</v>
+      </c>
+      <c r="C128" t="s">
+        <v>264</v>
+      </c>
+      <c r="D128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>201</v>
+      </c>
+      <c r="B129" t="s">
+        <v>124</v>
+      </c>
+      <c r="C129" t="s">
+        <v>52</v>
+      </c>
+      <c r="D129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>202</v>
+      </c>
+      <c r="B130" t="s">
+        <v>125</v>
+      </c>
+      <c r="C130" t="s">
+        <v>53</v>
+      </c>
+      <c r="D130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>220</v>
+      </c>
+      <c r="B131" t="s">
+        <v>142</v>
+      </c>
+      <c r="C131" t="s">
+        <v>71</v>
+      </c>
+      <c r="D131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>221</v>
+      </c>
+      <c r="B132" t="s">
+        <v>143</v>
+      </c>
+      <c r="C132" t="s">
+        <v>72</v>
+      </c>
+      <c r="D132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>2344</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2348</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2343</v>
+      </c>
+      <c r="D133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>186</v>
+      </c>
+      <c r="B134" t="s">
+        <v>111</v>
+      </c>
+      <c r="C134" t="s">
+        <v>35</v>
+      </c>
+      <c r="D134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>187</v>
+      </c>
+      <c r="B135" t="s">
+        <v>112</v>
+      </c>
+      <c r="C135" t="s">
+        <v>36</v>
+      </c>
+      <c r="D135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C136" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C137" t="s">
+        <v>2337</v>
+      </c>
+      <c r="D137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>2369</v>
+      </c>
+      <c r="B138" t="s">
+        <v>2370</v>
+      </c>
+      <c r="C138" t="s">
+        <v>2371</v>
+      </c>
+      <c r="D138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>2275</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2279</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>2277</v>
+      </c>
+      <c r="B140" t="s">
+        <v>2280</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D140" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D140">
+    <sortCondition ref="A2:A140"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changes for Fly deployment
</commit_message>
<xml_diff>
--- a/reference/reference.xlsx
+++ b/reference/reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Programming/Python/Degenreur/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF53D27-0E4C-344F-8892-126F39228035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502F2790-FBF2-DD43-80F7-8A86AB40CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="17340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Female pronouns" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3097" uniqueCount="2429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="2438">
   <si>
     <t>Original</t>
   </si>
@@ -7310,6 +7310,33 @@
   </si>
   <si>
     <t>abbesses</t>
+  </si>
+  <si>
+    <t>countrywoman</t>
+  </si>
+  <si>
+    <t>countryfolk</t>
+  </si>
+  <si>
+    <t>countryman</t>
+  </si>
+  <si>
+    <t>countrywomen</t>
+  </si>
+  <si>
+    <t>countrymen</t>
+  </si>
+  <si>
+    <t>lordship</t>
+  </si>
+  <si>
+    <t>lord-ladyship</t>
+  </si>
+  <si>
+    <t>ladyshop</t>
+  </si>
+  <si>
+    <t>ladyship</t>
   </si>
 </sst>
 </file>
@@ -7368,12 +7395,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7678,10 +7704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A82" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8086,13 +8112,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>2429</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>2430</v>
       </c>
       <c r="C29" t="s">
-        <v>216</v>
+        <v>2431</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -8100,13 +8126,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>2432</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>2430</v>
       </c>
       <c r="C30" t="s">
-        <v>217</v>
+        <v>2433</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -8114,13 +8140,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>2363</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>177</v>
+        <v>216</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -8128,13 +8154,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>2360</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
-        <v>2356</v>
+        <v>217</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -8142,13 +8168,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>2363</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -8156,13 +8182,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>2360</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>2356</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -8170,13 +8196,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>2361</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -8184,13 +8210,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>2345</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>2350</v>
+        <v>125</v>
       </c>
       <c r="C36" t="s">
-        <v>2346</v>
+        <v>202</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -8198,13 +8224,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>2361</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>230</v>
+        <v>184</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -8212,13 +8238,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>2352</v>
+        <v>2345</v>
       </c>
       <c r="B38" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
       <c r="C38" t="s">
-        <v>2367</v>
+        <v>2346</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -8226,13 +8252,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>2240</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>2239</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
-        <v>2238</v>
+        <v>230</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -8240,13 +8266,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>2243</v>
+        <v>2352</v>
       </c>
       <c r="B40" t="s">
-        <v>2242</v>
+        <v>2352</v>
       </c>
       <c r="C40" t="s">
-        <v>2241</v>
+        <v>2367</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -8254,13 +8280,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>2334</v>
+        <v>2240</v>
       </c>
       <c r="B41" t="s">
-        <v>2336</v>
+        <v>2239</v>
       </c>
       <c r="C41" t="s">
-        <v>2335</v>
+        <v>2238</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -8268,13 +8294,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>2373</v>
+        <v>2243</v>
       </c>
       <c r="B42" t="s">
-        <v>2370</v>
+        <v>2242</v>
       </c>
       <c r="C42" t="s">
-        <v>2372</v>
+        <v>2241</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -8282,13 +8308,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>2337</v>
+        <v>2334</v>
       </c>
       <c r="B43" t="s">
         <v>2336</v>
       </c>
       <c r="C43" t="s">
-        <v>2338</v>
+        <v>2335</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -8296,13 +8322,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>2371</v>
+        <v>2373</v>
       </c>
       <c r="B44" t="s">
         <v>2370</v>
       </c>
       <c r="C44" t="s">
-        <v>2369</v>
+        <v>2372</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -8310,13 +8336,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>2337</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>2336</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>2338</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -8324,13 +8350,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>2252</v>
+        <v>2371</v>
       </c>
       <c r="B46" t="s">
-        <v>2251</v>
+        <v>2370</v>
       </c>
       <c r="C46" t="s">
-        <v>2250</v>
+        <v>2369</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -8338,13 +8364,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>2332</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>2333</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>2250</v>
+        <v>121</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -8352,13 +8378,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>2246</v>
+        <v>2252</v>
       </c>
       <c r="B48" t="s">
-        <v>2245</v>
+        <v>2251</v>
       </c>
       <c r="C48" t="s">
-        <v>2244</v>
+        <v>2250</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -8366,13 +8392,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>2248</v>
+        <v>2332</v>
       </c>
       <c r="B49" t="s">
-        <v>2249</v>
+        <v>2333</v>
       </c>
       <c r="C49" t="s">
-        <v>2247</v>
+        <v>2250</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -8380,13 +8406,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>2246</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>2245</v>
       </c>
       <c r="C50" t="s">
-        <v>178</v>
+        <v>2244</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -8394,13 +8420,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>2248</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>2249</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>2247</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -8408,10 +8434,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>257</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
         <v>178</v>
@@ -8422,13 +8448,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -8436,13 +8462,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
       <c r="C54" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -8450,13 +8476,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -8464,13 +8490,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -8478,13 +8504,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>2318</v>
+        <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>2317</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>2316</v>
+        <v>180</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -8492,13 +8518,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>2310</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>2312</v>
+        <v>106</v>
       </c>
       <c r="C58" t="s">
-        <v>2311</v>
+        <v>181</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -8506,13 +8532,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>2377</v>
+        <v>2318</v>
       </c>
       <c r="B59" t="s">
-        <v>2379</v>
+        <v>2317</v>
       </c>
       <c r="C59" t="s">
-        <v>2378</v>
+        <v>2316</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -8520,13 +8546,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>2310</v>
       </c>
       <c r="B60" t="s">
-        <v>258</v>
+        <v>2312</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>2311</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -8534,13 +8560,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>2377</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>2379</v>
       </c>
       <c r="C61" t="s">
-        <v>203</v>
+        <v>2378</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -8548,13 +8574,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
       <c r="C62" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
@@ -8562,13 +8588,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>2296</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>2297</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>2295</v>
+        <v>203</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -8576,13 +8602,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>2298</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>2299</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>2300</v>
+        <v>204</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -8590,13 +8616,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>2296</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>2297</v>
       </c>
       <c r="C65" t="s">
-        <v>199</v>
+        <v>2295</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -8604,13 +8630,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>51</v>
+        <v>2298</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>2299</v>
       </c>
       <c r="C66" t="s">
-        <v>200</v>
+        <v>2300</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -8618,13 +8644,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C67" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -8632,13 +8658,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -8646,13 +8672,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -8660,13 +8686,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B70" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C70" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -8674,13 +8700,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -8688,13 +8714,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C72" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -8702,13 +8728,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C73" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D73" t="b">
         <v>1</v>
@@ -8716,13 +8742,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C74" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -8730,13 +8756,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C75" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
@@ -8744,13 +8770,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B76" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
@@ -8758,13 +8784,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
       <c r="C77" t="s">
-        <v>223</v>
+        <v>162</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
@@ -8772,13 +8798,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B78" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
@@ -8786,13 +8812,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="B79" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="C79" t="s">
-        <v>163</v>
+        <v>223</v>
       </c>
       <c r="D79" t="b">
         <v>1</v>
@@ -8800,13 +8826,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -8814,13 +8840,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>225</v>
+        <v>163</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
@@ -8828,13 +8854,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>2398</v>
+        <v>75</v>
       </c>
       <c r="B82" t="s">
-        <v>2402</v>
+        <v>146</v>
       </c>
       <c r="C82" t="s">
-        <v>2399</v>
+        <v>224</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -8842,13 +8868,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>2400</v>
+        <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>2402</v>
+        <v>147</v>
       </c>
       <c r="C83" t="s">
-        <v>2401</v>
+        <v>225</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -8856,13 +8882,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>34</v>
+        <v>2398</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>2402</v>
       </c>
       <c r="C84" t="s">
-        <v>185</v>
+        <v>2399</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
@@ -8870,13 +8896,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>33</v>
+        <v>2400</v>
       </c>
       <c r="B85" t="s">
-        <v>109</v>
+        <v>2402</v>
       </c>
       <c r="C85" t="s">
-        <v>184</v>
+        <v>2401</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -8884,13 +8910,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>2313</v>
+        <v>34</v>
       </c>
       <c r="B86" t="s">
-        <v>2319</v>
+        <v>110</v>
       </c>
       <c r="C86" t="s">
-        <v>2320</v>
+        <v>185</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -8898,13 +8924,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>2314</v>
+        <v>33</v>
       </c>
       <c r="B87" t="s">
-        <v>2319</v>
+        <v>109</v>
       </c>
       <c r="C87" t="s">
-        <v>2320</v>
+        <v>184</v>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -8912,13 +8938,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>2292</v>
+        <v>2313</v>
       </c>
       <c r="B88" t="s">
-        <v>2293</v>
+        <v>2319</v>
       </c>
       <c r="C88" t="s">
-        <v>2294</v>
+        <v>2320</v>
       </c>
       <c r="D88" t="b">
         <v>1</v>
@@ -8926,13 +8952,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>2287</v>
+        <v>2314</v>
       </c>
       <c r="B89" t="s">
-        <v>2289</v>
+        <v>2319</v>
       </c>
       <c r="C89" t="s">
-        <v>2288</v>
+        <v>2320</v>
       </c>
       <c r="D89" t="b">
         <v>1</v>
@@ -8940,13 +8966,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>2290</v>
+        <v>2437</v>
       </c>
       <c r="B90" t="s">
-        <v>257</v>
+        <v>2435</v>
       </c>
       <c r="C90" t="s">
-        <v>2291</v>
+        <v>2434</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -8954,13 +8980,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>2261</v>
+        <v>2292</v>
       </c>
       <c r="B91" t="s">
-        <v>2262</v>
+        <v>2293</v>
       </c>
       <c r="C91" t="s">
-        <v>2263</v>
+        <v>2294</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -8968,13 +8994,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>24</v>
+        <v>2287</v>
       </c>
       <c r="B92" t="s">
-        <v>2329</v>
+        <v>2289</v>
       </c>
       <c r="C92" t="s">
-        <v>177</v>
+        <v>2288</v>
       </c>
       <c r="D92" t="b">
         <v>1</v>
@@ -8982,13 +9008,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>23</v>
+        <v>2290</v>
       </c>
       <c r="B93" t="s">
-        <v>2328</v>
+        <v>257</v>
       </c>
       <c r="C93" t="s">
-        <v>177</v>
+        <v>2291</v>
       </c>
       <c r="D93" t="b">
         <v>1</v>
@@ -8996,13 +9022,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>22</v>
+        <v>2261</v>
       </c>
       <c r="B94" t="s">
-        <v>2328</v>
+        <v>2262</v>
       </c>
       <c r="C94" t="s">
-        <v>176</v>
+        <v>2263</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -9010,13 +9036,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B95" t="s">
-        <v>2253</v>
+        <v>2329</v>
       </c>
       <c r="C95" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -9024,13 +9050,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>2331</v>
+        <v>23</v>
       </c>
       <c r="B96" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="C96" t="s">
-        <v>243</v>
+        <v>177</v>
       </c>
       <c r="D96" t="b">
         <v>1</v>
@@ -9038,13 +9064,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>264</v>
+        <v>22</v>
       </c>
       <c r="B97" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="C97" t="s">
-        <v>243</v>
+        <v>176</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -9052,13 +9078,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>2362</v>
+        <v>22</v>
       </c>
       <c r="B98" t="s">
-        <v>109</v>
+        <v>2253</v>
       </c>
       <c r="C98" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D98" t="b">
         <v>1</v>
@@ -9066,13 +9092,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>2393</v>
+        <v>2331</v>
       </c>
       <c r="B99" t="s">
-        <v>2394</v>
+        <v>2330</v>
       </c>
       <c r="C99" t="s">
-        <v>2392</v>
+        <v>243</v>
       </c>
       <c r="D99" t="b">
         <v>1</v>
@@ -9080,13 +9106,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>2395</v>
+        <v>264</v>
       </c>
       <c r="B100" t="s">
-        <v>2396</v>
+        <v>2330</v>
       </c>
       <c r="C100" t="s">
-        <v>2397</v>
+        <v>243</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -9094,13 +9120,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>2301</v>
+        <v>2362</v>
       </c>
       <c r="B101" t="s">
-        <v>2302</v>
+        <v>109</v>
       </c>
       <c r="C101" t="s">
-        <v>2303</v>
+        <v>184</v>
       </c>
       <c r="D101" t="b">
         <v>1</v>
@@ -9108,13 +9134,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>29</v>
+        <v>2393</v>
       </c>
       <c r="B102" t="s">
-        <v>107</v>
+        <v>2394</v>
       </c>
       <c r="C102" t="s">
-        <v>182</v>
+        <v>2392</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -9122,13 +9148,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>30</v>
+        <v>2395</v>
       </c>
       <c r="B103" t="s">
-        <v>108</v>
+        <v>2396</v>
       </c>
       <c r="C103" t="s">
-        <v>183</v>
+        <v>2397</v>
       </c>
       <c r="D103" t="b">
         <v>1</v>
@@ -9136,13 +9162,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>2304</v>
+        <v>2301</v>
       </c>
       <c r="B104" t="s">
-        <v>2305</v>
+        <v>2302</v>
       </c>
       <c r="C104" t="s">
-        <v>2306</v>
+        <v>2303</v>
       </c>
       <c r="D104" t="b">
         <v>1</v>
@@ -9150,13 +9176,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B105" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -9164,13 +9190,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B106" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="D106" t="b">
         <v>1</v>
@@ -9178,13 +9204,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>2353</v>
+        <v>2304</v>
       </c>
       <c r="B107" t="s">
-        <v>2354</v>
+        <v>2305</v>
       </c>
       <c r="C107" t="s">
-        <v>2355</v>
+        <v>2306</v>
       </c>
       <c r="D107" t="b">
         <v>1</v>
@@ -9192,27 +9218,27 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>2175</v>
+        <v>12</v>
       </c>
       <c r="B108" t="s">
-        <v>2176</v>
+        <v>100</v>
       </c>
       <c r="C108" t="s">
-        <v>2177</v>
+        <v>168</v>
       </c>
       <c r="D108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B109" t="s">
-        <v>2329</v>
+        <v>100</v>
       </c>
       <c r="C109" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D109" t="b">
         <v>1</v>
@@ -9220,13 +9246,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>2353</v>
       </c>
       <c r="B110" t="s">
-        <v>2329</v>
+        <v>2354</v>
       </c>
       <c r="C110" t="s">
-        <v>175</v>
+        <v>2355</v>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -9234,27 +9260,27 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>19</v>
+        <v>2175</v>
       </c>
       <c r="B111" t="s">
-        <v>104</v>
+        <v>2176</v>
       </c>
       <c r="C111" t="s">
-        <v>175</v>
+        <v>2177</v>
       </c>
       <c r="D111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>2266</v>
+        <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>2268</v>
+        <v>2329</v>
       </c>
       <c r="C112" t="s">
-        <v>2267</v>
+        <v>175</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -9262,13 +9288,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>2410</v>
+        <v>20</v>
       </c>
       <c r="B113" t="s">
-        <v>100</v>
+        <v>2329</v>
       </c>
       <c r="C113" t="s">
-        <v>2411</v>
+        <v>175</v>
       </c>
       <c r="D113" t="b">
         <v>1</v>
@@ -9276,13 +9302,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>2417</v>
+        <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>2413</v>
+        <v>104</v>
       </c>
       <c r="C114" t="s">
-        <v>2418</v>
+        <v>175</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -9290,13 +9316,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>2266</v>
       </c>
       <c r="B115" t="s">
-        <v>100</v>
+        <v>2268</v>
       </c>
       <c r="C115" t="s">
-        <v>169</v>
+        <v>2267</v>
       </c>
       <c r="D115" t="b">
         <v>1</v>
@@ -9304,13 +9330,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>2412</v>
+        <v>2410</v>
       </c>
       <c r="B116" t="s">
-        <v>2413</v>
+        <v>100</v>
       </c>
       <c r="C116" t="s">
-        <v>2414</v>
+        <v>2411</v>
       </c>
       <c r="D116" t="b">
         <v>1</v>
@@ -9318,13 +9344,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>2415</v>
+        <v>2417</v>
       </c>
       <c r="B117" t="s">
         <v>2413</v>
       </c>
       <c r="C117" t="s">
-        <v>2416</v>
+        <v>2418</v>
       </c>
       <c r="D117" t="b">
         <v>1</v>
@@ -9332,13 +9358,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B118" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C118" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D118" t="b">
         <v>1</v>
@@ -9346,13 +9372,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>2282</v>
+        <v>2412</v>
       </c>
       <c r="B119" t="s">
-        <v>2283</v>
+        <v>2413</v>
       </c>
       <c r="C119" t="s">
-        <v>2281</v>
+        <v>2414</v>
       </c>
       <c r="D119" t="b">
         <v>1</v>
@@ -9360,13 +9386,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>2415</v>
       </c>
       <c r="B120" t="s">
-        <v>99</v>
+        <v>2413</v>
       </c>
       <c r="C120" t="s">
-        <v>167</v>
+        <v>2416</v>
       </c>
       <c r="D120" t="b">
         <v>1</v>
@@ -9374,13 +9400,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C121" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D121" t="b">
         <v>1</v>
@@ -9388,13 +9414,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>37</v>
+        <v>2282</v>
       </c>
       <c r="B122" t="s">
-        <v>113</v>
+        <v>2283</v>
       </c>
       <c r="C122" t="s">
-        <v>188</v>
+        <v>2281</v>
       </c>
       <c r="D122" t="b">
         <v>1</v>
@@ -9402,13 +9428,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C123" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="D123" t="b">
         <v>1</v>
@@ -9416,13 +9442,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>2403</v>
+        <v>18</v>
       </c>
       <c r="B124" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="C124" t="s">
-        <v>2404</v>
+        <v>174</v>
       </c>
       <c r="D124" t="b">
         <v>1</v>
@@ -9430,13 +9456,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>2405</v>
+        <v>37</v>
       </c>
       <c r="B125" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="C125" t="s">
-        <v>2406</v>
+        <v>188</v>
       </c>
       <c r="D125" t="b">
         <v>1</v>
@@ -9444,13 +9470,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B126" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="C126" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="D126" t="b">
         <v>1</v>
@@ -9458,13 +9484,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>82</v>
+        <v>2403</v>
       </c>
       <c r="B127" t="s">
         <v>151</v>
       </c>
       <c r="C127" t="s">
-        <v>231</v>
+        <v>2404</v>
       </c>
       <c r="D127" t="b">
         <v>1</v>
@@ -9472,13 +9498,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>83</v>
+        <v>2405</v>
       </c>
       <c r="B128" t="s">
         <v>152</v>
       </c>
       <c r="C128" t="s">
-        <v>232</v>
+        <v>2406</v>
       </c>
       <c r="D128" t="b">
         <v>1</v>
@@ -9486,13 +9512,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B129" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C129" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D129" t="b">
         <v>1</v>
@@ -9500,13 +9526,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B130" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="C130" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="D130" t="b">
         <v>1</v>
@@ -9514,13 +9540,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>2342</v>
+        <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>2349</v>
+        <v>152</v>
       </c>
       <c r="C131" t="s">
-        <v>2341</v>
+        <v>232</v>
       </c>
       <c r="D131" t="b">
         <v>1</v>
@@ -9528,13 +9554,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="B132" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="D132" t="b">
         <v>1</v>
@@ -9542,13 +9568,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="B133" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="D133" t="b">
         <v>1</v>
@@ -9556,13 +9582,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>89</v>
+        <v>2342</v>
       </c>
       <c r="B134" t="s">
-        <v>2178</v>
+        <v>2349</v>
       </c>
       <c r="C134" t="s">
-        <v>237</v>
+        <v>2341</v>
       </c>
       <c r="D134" t="b">
         <v>1</v>
@@ -9570,13 +9596,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>2256</v>
+        <v>90</v>
       </c>
       <c r="B135" t="s">
-        <v>2255</v>
+        <v>159</v>
       </c>
       <c r="C135" t="s">
-        <v>2254</v>
+        <v>238</v>
       </c>
       <c r="D135" t="b">
         <v>1</v>
@@ -9584,13 +9610,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="B136" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="C136" t="s">
-        <v>161</v>
+        <v>239</v>
       </c>
       <c r="D136" t="b">
         <v>1</v>
@@ -9598,13 +9624,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>2257</v>
+        <v>89</v>
       </c>
       <c r="B137" t="s">
-        <v>2258</v>
+        <v>2178</v>
       </c>
       <c r="C137" t="s">
-        <v>2259</v>
+        <v>237</v>
       </c>
       <c r="D137" t="b">
         <v>1</v>
@@ -9612,13 +9638,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>2260</v>
+        <v>2256</v>
       </c>
       <c r="B138" t="s">
-        <v>2258</v>
+        <v>2255</v>
       </c>
       <c r="C138" t="s">
-        <v>2259</v>
+        <v>2254</v>
       </c>
       <c r="D138" t="b">
         <v>1</v>
@@ -9626,13 +9652,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B139" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C139" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D139" t="b">
         <v>1</v>
@@ -9640,13 +9666,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>15</v>
+        <v>2257</v>
       </c>
       <c r="B140" t="s">
-        <v>101</v>
+        <v>2258</v>
       </c>
       <c r="C140" t="s">
-        <v>171</v>
+        <v>2259</v>
       </c>
       <c r="D140" t="b">
         <v>1</v>
@@ -9654,13 +9680,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>2309</v>
+        <v>2260</v>
       </c>
       <c r="B141" t="s">
-        <v>2308</v>
+        <v>2258</v>
       </c>
       <c r="C141" t="s">
-        <v>2307</v>
+        <v>2259</v>
       </c>
       <c r="D141" t="b">
         <v>1</v>
@@ -9668,13 +9694,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C142" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D142" t="b">
         <v>1</v>
@@ -9682,13 +9708,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="B143" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="C143" t="s">
-        <v>220</v>
+        <v>171</v>
       </c>
       <c r="D143" t="b">
         <v>1</v>
@@ -9696,13 +9722,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>72</v>
+        <v>2309</v>
       </c>
       <c r="B144" t="s">
-        <v>143</v>
+        <v>2308</v>
       </c>
       <c r="C144" t="s">
-        <v>221</v>
+        <v>2307</v>
       </c>
       <c r="D144" t="b">
         <v>1</v>
@@ -9710,13 +9736,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>2343</v>
+        <v>16</v>
       </c>
       <c r="B145" t="s">
-        <v>2348</v>
+        <v>102</v>
       </c>
       <c r="C145" t="s">
-        <v>2344</v>
+        <v>172</v>
       </c>
       <c r="D145" t="b">
         <v>1</v>
@@ -9724,13 +9750,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>2384</v>
+        <v>71</v>
       </c>
       <c r="B146" t="s">
-        <v>2386</v>
+        <v>142</v>
       </c>
       <c r="C146" t="s">
-        <v>2385</v>
+        <v>220</v>
       </c>
       <c r="D146" t="b">
         <v>1</v>
@@ -9738,13 +9764,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>2323</v>
+        <v>72</v>
       </c>
       <c r="B147" t="s">
-        <v>2324</v>
+        <v>143</v>
       </c>
       <c r="C147" t="s">
-        <v>2322</v>
+        <v>221</v>
       </c>
       <c r="D147" t="b">
         <v>1</v>
@@ -9752,13 +9778,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>2321</v>
+        <v>2343</v>
       </c>
       <c r="B148" t="s">
-        <v>2324</v>
+        <v>2348</v>
       </c>
       <c r="C148" t="s">
-        <v>2322</v>
+        <v>2344</v>
       </c>
       <c r="D148" t="b">
         <v>1</v>
@@ -9766,13 +9792,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>77</v>
+        <v>2384</v>
       </c>
       <c r="B149" t="s">
-        <v>148</v>
+        <v>2386</v>
       </c>
       <c r="C149" t="s">
-        <v>226</v>
+        <v>2385</v>
       </c>
       <c r="D149" t="b">
         <v>1</v>
@@ -9780,13 +9806,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>78</v>
+        <v>2323</v>
       </c>
       <c r="B150" t="s">
-        <v>148</v>
+        <v>2324</v>
       </c>
       <c r="C150" t="s">
-        <v>227</v>
+        <v>2322</v>
       </c>
       <c r="D150" t="b">
         <v>1</v>
@@ -9794,13 +9820,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>47</v>
+        <v>2321</v>
       </c>
       <c r="B151" t="s">
-        <v>119</v>
+        <v>2324</v>
       </c>
       <c r="C151" t="s">
-        <v>197</v>
+        <v>2322</v>
       </c>
       <c r="D151" t="b">
         <v>1</v>
@@ -9808,13 +9834,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>2276</v>
+        <v>77</v>
       </c>
       <c r="B152" t="s">
-        <v>2279</v>
+        <v>148</v>
       </c>
       <c r="C152" t="s">
-        <v>2275</v>
+        <v>226</v>
       </c>
       <c r="D152" t="b">
         <v>1</v>
@@ -9822,13 +9848,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>2278</v>
+        <v>78</v>
       </c>
       <c r="B153" t="s">
-        <v>2280</v>
+        <v>148</v>
       </c>
       <c r="C153" t="s">
-        <v>2277</v>
+        <v>227</v>
       </c>
       <c r="D153" t="b">
         <v>1</v>
@@ -9836,13 +9862,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B154" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C154" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D154" t="b">
         <v>1</v>
@@ -9850,13 +9876,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>8</v>
+        <v>2276</v>
       </c>
       <c r="B155" t="s">
-        <v>96</v>
+        <v>2279</v>
       </c>
       <c r="C155" t="s">
-        <v>164</v>
+        <v>2275</v>
       </c>
       <c r="D155" t="b">
         <v>1</v>
@@ -9864,13 +9890,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>2375</v>
+        <v>2278</v>
       </c>
       <c r="B156" t="s">
-        <v>2376</v>
+        <v>2280</v>
       </c>
       <c r="C156" t="s">
-        <v>2374</v>
+        <v>2277</v>
       </c>
       <c r="D156" t="b">
         <v>1</v>
@@ -9878,13 +9904,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>2359</v>
+        <v>48</v>
       </c>
       <c r="B157" t="s">
-        <v>2336</v>
+        <v>120</v>
       </c>
       <c r="C157" t="s">
-        <v>2358</v>
+        <v>198</v>
       </c>
       <c r="D157" t="b">
         <v>1</v>
@@ -9892,13 +9918,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>2325</v>
+        <v>8</v>
       </c>
       <c r="B158" t="s">
-        <v>2327</v>
+        <v>96</v>
       </c>
       <c r="C158" t="s">
-        <v>2326</v>
+        <v>164</v>
       </c>
       <c r="D158" t="b">
         <v>1</v>
@@ -9906,13 +9932,13 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>2325</v>
+        <v>2375</v>
       </c>
       <c r="B159" t="s">
-        <v>2336</v>
+        <v>2376</v>
       </c>
       <c r="C159" t="s">
-        <v>2380</v>
+        <v>2374</v>
       </c>
       <c r="D159" t="b">
         <v>1</v>
@@ -9920,21 +9946,63 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>2359</v>
+      </c>
+      <c r="B160" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2358</v>
+      </c>
+      <c r="D160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B161" t="s">
+        <v>2327</v>
+      </c>
+      <c r="C161" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B162" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C162" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>9</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B163" t="s">
         <v>97</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C163" t="s">
         <v>165</v>
       </c>
-      <c r="D160" t="b">
+      <c r="D163" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D160">
-    <sortCondition ref="A4:A160"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D163">
+    <sortCondition ref="A4:A163"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9942,10 +10010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9984,17 +10052,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>219</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="2" t="b">
+      <c r="D3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10420,13 +10488,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>216</v>
+        <v>2431</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>2430</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>2429</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -10434,13 +10502,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>217</v>
+        <v>2433</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>2430</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>2432</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -10448,13 +10516,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>2411</v>
+        <v>216</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
-        <v>2410</v>
+        <v>67</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -10462,13 +10530,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>2418</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
-        <v>2413</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>2417</v>
+        <v>68</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -10476,13 +10544,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>2411</v>
       </c>
       <c r="B38" t="s">
         <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>2410</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -10490,13 +10558,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>2414</v>
+        <v>2418</v>
       </c>
       <c r="B39" t="s">
         <v>2413</v>
       </c>
       <c r="C39" t="s">
-        <v>2412</v>
+        <v>2417</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -10504,13 +10572,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>2416</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
-        <v>2413</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>2415</v>
+        <v>13</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -10518,13 +10586,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>230</v>
+        <v>2414</v>
       </c>
       <c r="B41" t="s">
-        <v>149</v>
+        <v>2413</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>2412</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -10532,13 +10600,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>247</v>
+        <v>2416</v>
       </c>
       <c r="B42" t="s">
-        <v>150</v>
+        <v>2413</v>
       </c>
       <c r="C42" t="s">
-        <v>266</v>
+        <v>2415</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -10546,13 +10614,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>2238</v>
+        <v>230</v>
       </c>
       <c r="B43" t="s">
-        <v>2239</v>
+        <v>149</v>
       </c>
       <c r="C43" t="s">
-        <v>2240</v>
+        <v>81</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -10560,13 +10628,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>2241</v>
+        <v>247</v>
       </c>
       <c r="B44" t="s">
-        <v>2242</v>
+        <v>150</v>
       </c>
       <c r="C44" t="s">
-        <v>2243</v>
+        <v>266</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -10574,13 +10642,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>2238</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>2239</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>2240</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -10588,13 +10656,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>2281</v>
+        <v>2241</v>
       </c>
       <c r="B46" t="s">
-        <v>2283</v>
+        <v>2242</v>
       </c>
       <c r="C46" t="s">
-        <v>2282</v>
+        <v>2243</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -10602,13 +10670,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -10616,13 +10684,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>2385</v>
+        <v>2281</v>
       </c>
       <c r="B48" t="s">
-        <v>2386</v>
+        <v>2283</v>
       </c>
       <c r="C48" t="s">
-        <v>2384</v>
+        <v>2282</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -10630,13 +10698,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>2244</v>
+        <v>167</v>
       </c>
       <c r="B49" t="s">
-        <v>2245</v>
+        <v>99</v>
       </c>
       <c r="C49" t="s">
-        <v>2246</v>
+        <v>11</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -10644,13 +10712,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>2247</v>
+        <v>2385</v>
       </c>
       <c r="B50" t="s">
-        <v>2249</v>
+        <v>2386</v>
       </c>
       <c r="C50" t="s">
-        <v>2248</v>
+        <v>2384</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -10658,13 +10726,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>2420</v>
+        <v>2244</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>2245</v>
       </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>2246</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -10672,13 +10740,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>2419</v>
+        <v>2247</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>2249</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>2248</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -10686,13 +10754,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>2356</v>
+        <v>2420</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -10700,13 +10768,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>2419</v>
       </c>
       <c r="B54" t="s">
-        <v>2391</v>
+        <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -10714,13 +10782,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>2320</v>
+        <v>2356</v>
       </c>
       <c r="B55" t="s">
-        <v>2319</v>
+        <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>2314</v>
+        <v>33</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -10728,13 +10796,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B56" t="s">
         <v>2391</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -10742,13 +10810,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>2390</v>
+        <v>2320</v>
       </c>
       <c r="B57" t="s">
-        <v>2391</v>
+        <v>2319</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
+        <v>2314</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -10756,13 +10824,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>2295</v>
+        <v>185</v>
       </c>
       <c r="B58" t="s">
-        <v>2297</v>
+        <v>2391</v>
       </c>
       <c r="C58" t="s">
-        <v>2296</v>
+        <v>34</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -10770,13 +10838,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>199</v>
+        <v>2390</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>2391</v>
       </c>
       <c r="C59" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -10784,13 +10852,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>200</v>
+        <v>2295</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>2297</v>
       </c>
       <c r="C60" t="s">
-        <v>51</v>
+        <v>2296</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -10798,13 +10866,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>2300</v>
+        <v>199</v>
       </c>
       <c r="B61" t="s">
-        <v>2299</v>
+        <v>122</v>
       </c>
       <c r="C61" t="s">
-        <v>2298</v>
+        <v>50</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -10812,13 +10880,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
@@ -10826,13 +10894,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>204</v>
+        <v>2300</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>2299</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>2298</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -10840,13 +10908,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="B64" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -10854,13 +10922,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="C65" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -10868,13 +10936,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B66" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C66" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -10882,13 +10950,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B67" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -10896,13 +10964,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -10910,13 +10978,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -10924,13 +10992,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="B70" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -10938,13 +11006,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="B71" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C71" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -10952,13 +11020,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>2421</v>
+        <v>235</v>
       </c>
       <c r="B72" t="s">
-        <v>2424</v>
+        <v>156</v>
       </c>
       <c r="C72" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -10966,13 +11034,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>2422</v>
+        <v>236</v>
       </c>
       <c r="B73" t="s">
-        <v>2423</v>
+        <v>157</v>
       </c>
       <c r="C73" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D73" t="b">
         <v>1</v>
@@ -10980,13 +11048,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>248</v>
+        <v>2421</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>2424</v>
       </c>
       <c r="C74" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -10994,13 +11062,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>161</v>
+        <v>2422</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>2423</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
@@ -11008,13 +11076,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="B76" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C76" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
@@ -11022,13 +11090,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>223</v>
+        <v>161</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="C77" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
@@ -11036,13 +11104,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>2250</v>
+        <v>222</v>
       </c>
       <c r="B78" t="s">
-        <v>2251</v>
+        <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>2252</v>
+        <v>73</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
@@ -11050,13 +11118,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B79" t="s">
-        <v>255</v>
+        <v>145</v>
       </c>
       <c r="C79" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="D79" t="b">
         <v>1</v>
@@ -11064,13 +11132,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>2365</v>
+        <v>2250</v>
       </c>
       <c r="B80" t="s">
-        <v>2366</v>
+        <v>2251</v>
       </c>
       <c r="C80" t="s">
-        <v>2364</v>
+        <v>2252</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -11078,13 +11146,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>240</v>
       </c>
       <c r="B81" t="s">
-        <v>95</v>
+        <v>255</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
@@ -11092,13 +11160,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>162</v>
+        <v>2365</v>
       </c>
       <c r="B82" t="s">
-        <v>93</v>
+        <v>2366</v>
       </c>
       <c r="C82" t="s">
-        <v>5</v>
+        <v>2364</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -11106,13 +11174,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>2339</v>
+        <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>2351</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>2340</v>
+        <v>7</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -11120,13 +11188,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="C84" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
@@ -11134,13 +11202,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>225</v>
+        <v>2339</v>
       </c>
       <c r="B85" t="s">
-        <v>147</v>
+        <v>2351</v>
       </c>
       <c r="C85" t="s">
-        <v>76</v>
+        <v>2340</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -11148,13 +11216,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="C86" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -11162,13 +11230,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="C87" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -11176,13 +11244,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B88" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C88" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D88" t="b">
         <v>1</v>
@@ -11190,13 +11258,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C89" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D89" t="b">
         <v>1</v>
@@ -11204,13 +11272,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>2399</v>
+        <v>211</v>
       </c>
       <c r="B90" t="s">
-        <v>2402</v>
+        <v>134</v>
       </c>
       <c r="C90" t="s">
-        <v>2398</v>
+        <v>62</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -11218,13 +11286,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>2401</v>
+        <v>212</v>
       </c>
       <c r="B91" t="s">
-        <v>2402</v>
+        <v>135</v>
       </c>
       <c r="C91" t="s">
-        <v>2400</v>
+        <v>63</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -11232,13 +11300,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>2399</v>
       </c>
       <c r="B92" t="s">
-        <v>107</v>
+        <v>2402</v>
       </c>
       <c r="C92" t="s">
-        <v>25</v>
+        <v>2398</v>
       </c>
       <c r="D92" t="b">
         <v>1</v>
@@ -11246,13 +11314,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>244</v>
+        <v>2401</v>
       </c>
       <c r="B93" t="s">
-        <v>107</v>
+        <v>2402</v>
       </c>
       <c r="C93" t="s">
-        <v>31</v>
+        <v>2400</v>
       </c>
       <c r="D93" t="b">
         <v>1</v>
@@ -11260,13 +11328,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>245</v>
+        <v>182</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C94" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -11274,13 +11342,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="B95" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C95" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -11288,13 +11356,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>2294</v>
+        <v>245</v>
       </c>
       <c r="B96" t="s">
-        <v>2293</v>
+        <v>108</v>
       </c>
       <c r="C96" t="s">
-        <v>2292</v>
+        <v>32</v>
       </c>
       <c r="D96" t="b">
         <v>1</v>
@@ -11302,13 +11370,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>2263</v>
+        <v>183</v>
       </c>
       <c r="B97" t="s">
-        <v>2262</v>
+        <v>108</v>
       </c>
       <c r="C97" t="s">
-        <v>2261</v>
+        <v>26</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -11316,13 +11384,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>2236</v>
+        <v>2294</v>
       </c>
       <c r="B98" t="s">
-        <v>2237</v>
+        <v>2293</v>
       </c>
       <c r="C98" t="s">
-        <v>33</v>
+        <v>2292</v>
       </c>
       <c r="D98" t="b">
         <v>1</v>
@@ -11330,13 +11398,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>2387</v>
+        <v>2263</v>
       </c>
       <c r="B99" t="s">
-        <v>2389</v>
+        <v>2262</v>
       </c>
       <c r="C99" t="s">
-        <v>2388</v>
+        <v>2261</v>
       </c>
       <c r="D99" t="b">
         <v>1</v>
@@ -11344,13 +11412,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>2381</v>
+        <v>2236</v>
       </c>
       <c r="B100" t="s">
-        <v>2383</v>
+        <v>2237</v>
       </c>
       <c r="C100" t="s">
-        <v>2382</v>
+        <v>33</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -11358,13 +11426,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>2392</v>
+        <v>2434</v>
       </c>
       <c r="B101" t="s">
-        <v>2394</v>
+        <v>2435</v>
       </c>
       <c r="C101" t="s">
-        <v>2393</v>
+        <v>2436</v>
       </c>
       <c r="D101" t="b">
         <v>1</v>
@@ -11372,13 +11440,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>2397</v>
+        <v>2387</v>
       </c>
       <c r="B102" t="s">
-        <v>2396</v>
+        <v>2389</v>
       </c>
       <c r="C102" t="s">
-        <v>2395</v>
+        <v>2388</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -11386,13 +11454,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>249</v>
+        <v>2381</v>
       </c>
       <c r="B103" t="s">
-        <v>259</v>
+        <v>2383</v>
       </c>
       <c r="C103" t="s">
-        <v>267</v>
+        <v>2382</v>
       </c>
       <c r="D103" t="b">
         <v>1</v>
@@ -11400,13 +11468,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>250</v>
+        <v>2392</v>
       </c>
       <c r="B104" t="s">
-        <v>260</v>
+        <v>2394</v>
       </c>
       <c r="C104" t="s">
-        <v>268</v>
+        <v>2393</v>
       </c>
       <c r="D104" t="b">
         <v>1</v>
@@ -11414,13 +11482,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>2335</v>
+        <v>2397</v>
       </c>
       <c r="B105" t="s">
-        <v>2336</v>
+        <v>2396</v>
       </c>
       <c r="C105" t="s">
-        <v>2334</v>
+        <v>2395</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -11428,13 +11496,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>2372</v>
+        <v>249</v>
       </c>
       <c r="B106" t="s">
-        <v>2370</v>
+        <v>259</v>
       </c>
       <c r="C106" t="s">
-        <v>2373</v>
+        <v>267</v>
       </c>
       <c r="D106" t="b">
         <v>1</v>
@@ -11442,13 +11510,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>164</v>
+        <v>250</v>
       </c>
       <c r="B107" t="s">
-        <v>96</v>
+        <v>260</v>
       </c>
       <c r="C107" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="D107" t="b">
         <v>1</v>
@@ -11456,13 +11524,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>2357</v>
+        <v>2335</v>
       </c>
       <c r="B108" t="s">
         <v>2336</v>
       </c>
       <c r="C108" t="s">
-        <v>2325</v>
+        <v>2334</v>
       </c>
       <c r="D108" t="b">
         <v>1</v>
@@ -11470,13 +11538,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>2374</v>
+        <v>2372</v>
       </c>
       <c r="B109" t="s">
-        <v>2376</v>
+        <v>2370</v>
       </c>
       <c r="C109" t="s">
-        <v>2375</v>
+        <v>2373</v>
       </c>
       <c r="D109" t="b">
         <v>1</v>
@@ -11484,13 +11552,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>2358</v>
+        <v>164</v>
       </c>
       <c r="B110" t="s">
-        <v>2336</v>
+        <v>96</v>
       </c>
       <c r="C110" t="s">
-        <v>2359</v>
+        <v>8</v>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -11498,7 +11566,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>2326</v>
+        <v>2357</v>
       </c>
       <c r="B111" t="s">
         <v>2336</v>
@@ -11512,13 +11580,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>2380</v>
+        <v>2374</v>
       </c>
       <c r="B112" t="s">
-        <v>2336</v>
+        <v>2376</v>
       </c>
       <c r="C112" t="s">
-        <v>2325</v>
+        <v>2375</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -11526,13 +11594,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>2338</v>
+        <v>2358</v>
       </c>
       <c r="B113" t="s">
         <v>2336</v>
       </c>
       <c r="C113" t="s">
-        <v>2337</v>
+        <v>2359</v>
       </c>
       <c r="D113" t="b">
         <v>1</v>
@@ -11540,13 +11608,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>2284</v>
+        <v>2326</v>
       </c>
       <c r="B114" t="s">
-        <v>2285</v>
+        <v>2336</v>
       </c>
       <c r="C114" t="s">
-        <v>19</v>
+        <v>2325</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -11554,13 +11622,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>165</v>
+        <v>2380</v>
       </c>
       <c r="B115" t="s">
-        <v>97</v>
+        <v>2336</v>
       </c>
       <c r="C115" t="s">
-        <v>9</v>
+        <v>2325</v>
       </c>
       <c r="D115" t="b">
         <v>1</v>
@@ -11568,13 +11636,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>251</v>
+        <v>2338</v>
       </c>
       <c r="B116" t="s">
-        <v>261</v>
+        <v>2336</v>
       </c>
       <c r="C116" t="s">
-        <v>269</v>
+        <v>2337</v>
       </c>
       <c r="D116" t="b">
         <v>1</v>
@@ -11582,13 +11650,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>252</v>
+        <v>2284</v>
       </c>
       <c r="B117" t="s">
-        <v>261</v>
+        <v>2285</v>
       </c>
       <c r="C117" t="s">
-        <v>270</v>
+        <v>19</v>
       </c>
       <c r="D117" t="b">
         <v>1</v>
@@ -11596,13 +11664,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B118" t="s">
-        <v>2328</v>
+        <v>97</v>
       </c>
       <c r="C118" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D118" t="b">
         <v>1</v>
@@ -11610,13 +11678,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>2267</v>
+        <v>251</v>
       </c>
       <c r="B119" t="s">
-        <v>2330</v>
+        <v>261</v>
       </c>
       <c r="C119" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D119" t="b">
         <v>1</v>
@@ -11624,13 +11692,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>176</v>
+        <v>252</v>
       </c>
       <c r="B120" t="s">
-        <v>2253</v>
+        <v>261</v>
       </c>
       <c r="C120" t="s">
-        <v>22</v>
+        <v>270</v>
       </c>
       <c r="D120" t="b">
         <v>1</v>
@@ -11638,13 +11706,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
+        <v>2328</v>
       </c>
       <c r="C121" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D121" t="b">
         <v>1</v>
@@ -11652,13 +11720,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>2267</v>
       </c>
       <c r="B122" t="s">
-        <v>113</v>
+        <v>2330</v>
       </c>
       <c r="C122" t="s">
-        <v>37</v>
+        <v>264</v>
       </c>
       <c r="D122" t="b">
         <v>1</v>
@@ -11666,13 +11734,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>114</v>
+        <v>2253</v>
       </c>
       <c r="C123" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D123" t="b">
         <v>1</v>
@@ -11680,13 +11748,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>2404</v>
+        <v>174</v>
       </c>
       <c r="B124" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="C124" t="s">
-        <v>2403</v>
+        <v>18</v>
       </c>
       <c r="D124" t="b">
         <v>1</v>
@@ -11694,13 +11762,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>2406</v>
+        <v>188</v>
       </c>
       <c r="B125" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="C125" t="s">
-        <v>2405</v>
+        <v>37</v>
       </c>
       <c r="D125" t="b">
         <v>1</v>
@@ -11708,13 +11776,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="B126" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C126" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="D126" t="b">
         <v>1</v>
@@ -11722,13 +11790,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>2355</v>
+        <v>2404</v>
       </c>
       <c r="B127" t="s">
-        <v>2354</v>
+        <v>151</v>
       </c>
       <c r="C127" t="s">
-        <v>2353</v>
+        <v>2403</v>
       </c>
       <c r="D127" t="b">
         <v>1</v>
@@ -11736,13 +11804,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>170</v>
+        <v>2406</v>
       </c>
       <c r="B128" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="C128" t="s">
-        <v>14</v>
+        <v>2405</v>
       </c>
       <c r="D128" t="b">
         <v>1</v>
@@ -11750,27 +11818,27 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>241</v>
+        <v>168</v>
       </c>
       <c r="B129" t="s">
         <v>100</v>
       </c>
       <c r="C129" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>246</v>
+        <v>2355</v>
       </c>
       <c r="B130" t="s">
-        <v>137</v>
+        <v>2354</v>
       </c>
       <c r="C130" t="s">
-        <v>265</v>
+        <v>2353</v>
       </c>
       <c r="D130" t="b">
         <v>1</v>
@@ -11778,13 +11846,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="B131" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="C131" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="D131" t="b">
         <v>1</v>
@@ -11792,27 +11860,27 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="B132" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="C132" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="D132" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B133" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="C133" t="s">
-        <v>83</v>
+        <v>265</v>
       </c>
       <c r="D133" t="b">
         <v>1</v>
@@ -11820,13 +11888,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>2341</v>
+        <v>213</v>
       </c>
       <c r="B134" t="s">
-        <v>2349</v>
+        <v>137</v>
       </c>
       <c r="C134" t="s">
-        <v>2342</v>
+        <v>64</v>
       </c>
       <c r="D134" t="b">
         <v>1</v>
@@ -11834,13 +11902,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="B135" t="s">
-        <v>262</v>
+        <v>151</v>
       </c>
       <c r="C135" t="s">
-        <v>271</v>
+        <v>82</v>
       </c>
       <c r="D135" t="b">
         <v>1</v>
@@ -11848,13 +11916,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="B136" t="s">
-        <v>263</v>
+        <v>152</v>
       </c>
       <c r="C136" t="s">
-        <v>272</v>
+        <v>83</v>
       </c>
       <c r="D136" t="b">
         <v>1</v>
@@ -11862,13 +11930,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>238</v>
+        <v>2341</v>
       </c>
       <c r="B137" t="s">
-        <v>159</v>
+        <v>2349</v>
       </c>
       <c r="C137" t="s">
-        <v>90</v>
+        <v>2342</v>
       </c>
       <c r="D137" t="b">
         <v>1</v>
@@ -11876,13 +11944,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="B138" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="C138" t="s">
-        <v>91</v>
+        <v>271</v>
       </c>
       <c r="D138" t="b">
         <v>1</v>
@@ -11890,13 +11958,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="B139" t="s">
-        <v>2178</v>
+        <v>263</v>
       </c>
       <c r="C139" t="s">
-        <v>89</v>
+        <v>272</v>
       </c>
       <c r="D139" t="b">
         <v>1</v>
@@ -11904,13 +11972,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>2179</v>
+        <v>238</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C140" t="s">
-        <v>2180</v>
+        <v>90</v>
       </c>
       <c r="D140" t="b">
         <v>1</v>
@@ -11918,13 +11986,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>2254</v>
+        <v>239</v>
       </c>
       <c r="B141" t="s">
-        <v>2255</v>
+        <v>160</v>
       </c>
       <c r="C141" t="s">
-        <v>2256</v>
+        <v>91</v>
       </c>
       <c r="D141" t="b">
         <v>1</v>
@@ -11932,13 +12000,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>2346</v>
+        <v>237</v>
       </c>
       <c r="B142" t="s">
-        <v>2350</v>
+        <v>2178</v>
       </c>
       <c r="C142" t="s">
-        <v>2347</v>
+        <v>89</v>
       </c>
       <c r="D142" t="b">
         <v>1</v>
@@ -11946,13 +12014,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>2257</v>
+        <v>2179</v>
       </c>
       <c r="B143" t="s">
-        <v>2258</v>
+        <v>158</v>
       </c>
       <c r="C143" t="s">
-        <v>2259</v>
+        <v>2180</v>
       </c>
       <c r="D143" t="b">
         <v>1</v>
@@ -11960,13 +12028,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>2260</v>
+        <v>2254</v>
       </c>
       <c r="B144" t="s">
-        <v>2258</v>
+        <v>2255</v>
       </c>
       <c r="C144" t="s">
-        <v>2259</v>
+        <v>2256</v>
       </c>
       <c r="D144" t="b">
         <v>1</v>
@@ -11974,13 +12042,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>177</v>
+        <v>2346</v>
       </c>
       <c r="B145" t="s">
-        <v>2328</v>
+        <v>2350</v>
       </c>
       <c r="C145" t="s">
-        <v>23</v>
+        <v>2347</v>
       </c>
       <c r="D145" t="b">
         <v>1</v>
@@ -11988,13 +12056,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>243</v>
+        <v>2257</v>
       </c>
       <c r="B146" t="s">
-        <v>2330</v>
+        <v>2258</v>
       </c>
       <c r="C146" t="s">
-        <v>264</v>
+        <v>2259</v>
       </c>
       <c r="D146" t="b">
         <v>1</v>
@@ -12002,13 +12070,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>201</v>
+        <v>2260</v>
       </c>
       <c r="B147" t="s">
-        <v>124</v>
+        <v>2258</v>
       </c>
       <c r="C147" t="s">
-        <v>52</v>
+        <v>2259</v>
       </c>
       <c r="D147" t="b">
         <v>1</v>
@@ -12016,13 +12084,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="B148" t="s">
-        <v>125</v>
+        <v>2328</v>
       </c>
       <c r="C148" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D148" t="b">
         <v>1</v>
@@ -12030,13 +12098,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="B149" t="s">
-        <v>142</v>
+        <v>2330</v>
       </c>
       <c r="C149" t="s">
-        <v>71</v>
+        <v>264</v>
       </c>
       <c r="D149" t="b">
         <v>1</v>
@@ -12044,13 +12112,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="B150" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="C150" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D150" t="b">
         <v>1</v>
@@ -12058,13 +12126,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>2344</v>
+        <v>202</v>
       </c>
       <c r="B151" t="s">
-        <v>2348</v>
+        <v>125</v>
       </c>
       <c r="C151" t="s">
-        <v>2343</v>
+        <v>53</v>
       </c>
       <c r="D151" t="b">
         <v>1</v>
@@ -12072,13 +12140,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="B152" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C152" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D152" t="b">
         <v>1</v>
@@ -12086,13 +12154,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>187</v>
+        <v>221</v>
       </c>
       <c r="B153" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="C153" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D153" t="b">
         <v>1</v>
@@ -12100,13 +12168,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>2322</v>
+        <v>2344</v>
       </c>
       <c r="B154" t="s">
-        <v>2324</v>
+        <v>2348</v>
       </c>
       <c r="C154" t="s">
-        <v>2321</v>
+        <v>2343</v>
       </c>
       <c r="D154" t="b">
         <v>1</v>
@@ -12114,13 +12182,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>2368</v>
+        <v>186</v>
       </c>
       <c r="B155" t="s">
-        <v>2336</v>
+        <v>111</v>
       </c>
       <c r="C155" t="s">
-        <v>2337</v>
+        <v>35</v>
       </c>
       <c r="D155" t="b">
         <v>1</v>
@@ -12128,13 +12196,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>2369</v>
+        <v>187</v>
       </c>
       <c r="B156" t="s">
-        <v>2370</v>
+        <v>112</v>
       </c>
       <c r="C156" t="s">
-        <v>2371</v>
+        <v>36</v>
       </c>
       <c r="D156" t="b">
         <v>1</v>
@@ -12142,13 +12210,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>2275</v>
+        <v>2322</v>
       </c>
       <c r="B157" t="s">
-        <v>2279</v>
+        <v>2324</v>
       </c>
       <c r="C157" t="s">
-        <v>2276</v>
+        <v>2321</v>
       </c>
       <c r="D157" t="b">
         <v>1</v>
@@ -12156,21 +12224,63 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B158" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C158" t="s">
+        <v>2337</v>
+      </c>
+      <c r="D158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>2369</v>
+      </c>
+      <c r="B159" t="s">
+        <v>2370</v>
+      </c>
+      <c r="C159" t="s">
+        <v>2371</v>
+      </c>
+      <c r="D159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>2275</v>
+      </c>
+      <c r="B160" t="s">
+        <v>2279</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>2277</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B161" t="s">
         <v>2280</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C161" t="s">
         <v>2278</v>
       </c>
-      <c r="D158" t="b">
+      <c r="D161" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D158">
-    <sortCondition ref="A2:A158"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D161">
+    <sortCondition ref="A2:A161"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added tutorial videos to home page
</commit_message>
<xml_diff>
--- a/reference/reference.xlsx
+++ b/reference/reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Programming/Python/Degenreur/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502F2790-FBF2-DD43-80F7-8A86AB40CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE92A64F-9963-D141-BB48-11E2B9731B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="17340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="740" windowWidth="27300" windowHeight="17340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Female pronouns" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="2438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3119" uniqueCount="2442">
   <si>
     <t>Original</t>
   </si>
@@ -7337,6 +7337,18 @@
   </si>
   <si>
     <t>ladyship</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Gutenberg</t>
+  </si>
+  <si>
+    <t>Romeo</t>
+  </si>
+  <si>
+    <t>Juliet</t>
   </si>
 </sst>
 </file>
@@ -10012,7 +10024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+    <sheetView topLeftCell="A93" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
@@ -12288,10 +12300,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C806"/>
+  <dimension ref="A1:C807"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" topLeftCell="A798" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
+      <selection activeCell="A807" sqref="A807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17646,6 +17658,9 @@
       <c r="A618" t="s">
         <v>891</v>
       </c>
+      <c r="C618" t="s">
+        <v>2440</v>
+      </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A619" t="s">
@@ -18585,6 +18600,11 @@
     <row r="806" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A806" t="s">
         <v>1079</v>
+      </c>
+    </row>
+    <row r="807" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A807" t="s">
+        <v>2441</v>
       </c>
     </row>
   </sheetData>
@@ -18594,10 +18614,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B383"/>
+  <dimension ref="A1:B385"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="255" zoomScaleNormal="255" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView topLeftCell="A378" zoomScale="255" zoomScaleNormal="255" workbookViewId="0">
+      <selection activeCell="A385" sqref="A385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21121,6 +21141,16 @@
         <v>2093</v>
       </c>
     </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A384" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A385" t="s">
+        <v>2439</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>